<commit_message>
Prepare PT projects for minimal tests
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>Version</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>protothreads</t>
-  </si>
-  <si>
-    <t>k22ptmin_loop</t>
   </si>
   <si>
     <t>Tasks per second</t>
@@ -171,15 +168,9 @@
     <t>Optimisation</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>-O3</t>
   </si>
   <si>
-    <t>Results using on-board timer</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -192,7 +183,19 @@
     <t>-O0</t>
   </si>
   <si>
-    <t>Only change - each task's priority is set to 10. WHY?</t>
+    <t>Clock speed</t>
+  </si>
+  <si>
+    <t>Ops per us</t>
+  </si>
+  <si>
+    <t>k22ptmin_loop_only</t>
+  </si>
+  <si>
+    <t>Mean ops per task</t>
+  </si>
+  <si>
+    <t>Measurement of task switch time</t>
   </si>
 </sst>
 </file>
@@ -243,15 +246,14 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,8 +275,13 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -399,16 +406,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -424,14 +469,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,9 +491,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="6"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="5" builtinId="10"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
@@ -1186,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P23"/>
+  <dimension ref="B1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,38 +1256,40 @@
     <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="19"/>
+      <c r="C3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="16"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="M3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="12"/>
-    </row>
-    <row r="4" spans="2:16" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="20"/>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="2:15" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1246,29 +1300,32 @@
         <v>32</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="M4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O4" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1285,20 +1342,24 @@
       <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>41</v>
+      <c r="I5" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="M5">
-        <v>464810</v>
+        <v>464132</v>
       </c>
       <c r="N5" s="1">
         <f>10^6/M5</f>
-        <v>2.1514167079021536</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2.154559478768971</v>
+      </c>
+      <c r="O5" s="2">
+        <f>N5*$M$26</f>
+        <v>258.5471374522765</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -1307,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1316,17 +1377,21 @@
         <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="2">
-        <v>166000</v>
+        <v>40</v>
+      </c>
+      <c r="M6">
+        <v>949400</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" ref="N6:N23" si="0">10^6/M6</f>
-        <v>6.024096385542169</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+        <f>10^6/M6</f>
+        <v>1.0532968190436065</v>
+      </c>
+      <c r="O6" s="2">
+        <f>N6*$M$26</f>
+        <v>126.39561828523279</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>31</v>
       </c>
@@ -1346,12 +1411,21 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="M7">
+        <v>165108</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" ref="N7:N19" si="0">10^6/M7</f>
+        <v>6.0566417133028079</v>
+      </c>
+      <c r="O7" s="2">
+        <f>N7*$M$26</f>
+        <v>726.79700559633693</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>31</v>
       </c>
@@ -1371,12 +1445,21 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="M8">
+        <v>870240</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1491082919654347</v>
+      </c>
+      <c r="O8" s="2">
+        <f>N8*$M$26</f>
+        <v>137.89299503585218</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1399,17 +1482,21 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="M9">
-        <v>66736</v>
+        <v>136512</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
-        <v>14.984416207144569</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+        <v>7.3253633380215657</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" ref="O9:O11" si="1">N9*$M$26</f>
+        <v>879.04360056258793</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1426,23 +1513,27 @@
         <v>2</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="2">
-        <v>143063</v>
+        <v>40</v>
+      </c>
+      <c r="M10">
+        <v>122864</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
-        <v>6.9899275144516748</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+        <v>8.1390806094543553</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="1"/>
+        <v>976.68967313452265</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -1459,67 +1550,60 @@
         <v>2</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M11" s="2">
-        <v>138326</v>
+        <v>40</v>
+      </c>
+      <c r="M11">
+        <v>106028</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
-        <v>7.2292989025924266</v>
-      </c>
-      <c r="P11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+        <v>9.4314709322065866</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="1"/>
+        <v>1131.7765118647903</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M12" s="2">
-        <v>122148</v>
-      </c>
-      <c r="N12" s="1">
-        <f t="shared" si="0"/>
-        <v>8.1867897959851987</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -1527,13 +1611,16 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="I13" s="7"/>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -1552,96 +1639,148 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="2"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="17">
+        <v>45707</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="0"/>
+        <v>21.878486883847113</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="I16" s="7"/>
-      <c r="N16" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="17">
+        <v>53560</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="0"/>
+        <v>18.670649738610905</v>
+      </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-      <c r="I17" s="7"/>
-      <c r="N17" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7">
+        <v>2</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="M17" s="17">
+        <v>39118</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>25.563679124699625</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="N18" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="17">
+        <v>39450</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="0"/>
+        <v>25.34854245880862</v>
+      </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1666,156 +1805,62 @@
         <v>1</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19">
-        <v>45707</v>
+        <v>40</v>
+      </c>
+      <c r="M19" s="17">
+        <v>138323</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="0"/>
-        <v>21.878486883847113</v>
+        <v>7.2294556942807775</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20">
-        <v>53560</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" si="0"/>
-        <v>18.670649738610905</v>
-      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="G21" s="7">
-        <v>2</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="M21" s="9">
-        <v>39118</v>
-      </c>
-      <c r="N21" s="1">
-        <f t="shared" si="0"/>
-        <v>25.563679124699625</v>
-      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="1"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" s="9">
-        <v>39450</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" si="0"/>
-        <v>25.34854245880862</v>
-      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="1"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M23">
-        <v>138323</v>
-      </c>
-      <c r="N23" s="1">
-        <f t="shared" si="0"/>
-        <v>7.2294556942807775</v>
-      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>45</v>
+      </c>
+      <c r="M25">
+        <f>120*10^6</f>
+        <v>120000000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>46</v>
+      </c>
+      <c r="M26">
+        <f>M25/10^6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
CoMin with s/w timer completed
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>Version</t>
   </si>
@@ -202,7 +202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,15 +245,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,7 +270,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -444,16 +450,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -491,7 +499,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="6"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
@@ -504,10 +511,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="7" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
+    <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="7" builtinId="34"/>
+    <cellStyle name="20% - Accent4" xfId="8" builtinId="42"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="5" builtinId="10"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
@@ -1238,16 +1250,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O29"/>
+  <dimension ref="B1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="9" width="12" customWidth="1"/>
@@ -1283,11 +1295,11 @@
       <c r="I3" s="16"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="20"/>
-      <c r="O3" s="21"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="20"/>
     </row>
     <row r="4" spans="2:15" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -1319,7 +1331,7 @@
       <c r="N4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1353,7 +1365,7 @@
         <v>2.154559478768971</v>
       </c>
       <c r="O5" s="2">
-        <f>N5*$M$26</f>
+        <f>N5*$M$31</f>
         <v>258.5471374522765</v>
       </c>
     </row>
@@ -1386,8 +1398,8 @@
         <f>10^6/M6</f>
         <v>1.0532968190436065</v>
       </c>
-      <c r="O6" s="2">
-        <f>N6*$M$26</f>
+      <c r="O6" s="22">
+        <f>N6*$M$31</f>
         <v>126.39561828523279</v>
       </c>
     </row>
@@ -1421,7 +1433,7 @@
         <v>6.0566417133028079</v>
       </c>
       <c r="O7" s="2">
-        <f>N7*$M$26</f>
+        <f>N7*$M$31</f>
         <v>726.79700559633693</v>
       </c>
     </row>
@@ -1454,8 +1466,8 @@
         <f t="shared" si="0"/>
         <v>1.1491082919654347</v>
       </c>
-      <c r="O8" s="2">
-        <f>N8*$M$26</f>
+      <c r="O8" s="23">
+        <f>N8*$M$31</f>
         <v>137.89299503585218</v>
       </c>
     </row>
@@ -1491,8 +1503,8 @@
         <f t="shared" si="0"/>
         <v>7.3253633380215657</v>
       </c>
-      <c r="O9" s="2">
-        <f t="shared" ref="O9:O11" si="1">N9*$M$26</f>
+      <c r="O9" s="21">
+        <f t="shared" ref="O9:O11" si="1">N9*$M$31</f>
         <v>879.04360056258793</v>
       </c>
     </row>
@@ -1673,12 +1685,14 @@
       <c r="I15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M15" s="17">
-        <v>45707</v>
-      </c>
-      <c r="N15" s="1">
+      <c r="M15" s="2"/>
+      <c r="N15" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>21.878486883847113</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="2" t="e">
+        <f t="shared" ref="O15:O22" si="2">N15*$M$31</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
@@ -1706,15 +1720,17 @@
       <c r="I16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="17">
-        <v>53560</v>
-      </c>
-      <c r="N16" s="1">
+      <c r="M16" s="2"/>
+      <c r="N16" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>18.670649738610905</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -1741,15 +1757,17 @@
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="M17" s="17">
-        <v>39118</v>
-      </c>
-      <c r="N17" s="1">
+      <c r="M17" s="2"/>
+      <c r="N17" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>25.563679124699625</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -1774,15 +1792,17 @@
       <c r="I18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="17">
-        <v>39450</v>
-      </c>
-      <c r="N18" s="1">
+      <c r="M18" s="2"/>
+      <c r="N18" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>25.34854245880862</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1807,53 +1827,178 @@
       <c r="I19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M19" s="17">
-        <v>138323</v>
+      <c r="M19" s="2">
+        <v>138320</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="0"/>
-        <v>7.2294556942807775</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M21" s="2"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+        <v>7.2296124927703875</v>
+      </c>
+      <c r="O19" s="21">
+        <f t="shared" si="2"/>
+        <v>867.55349913244652</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="2">
+        <v>122144</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" ref="N20" si="3">10^6/M20</f>
+        <v>8.1870578988734604</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="2"/>
+        <v>982.44694786481523</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="2">
+        <v>108784</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" ref="N21" si="4">10^6/M21</f>
+        <v>9.1925283129872035</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="2"/>
+        <v>1103.1033975584644</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="M22" s="2"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N22" s="1" t="e">
+        <f t="shared" ref="N22" si="5">10^6/M22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I23" s="7"/>
       <c r="M23" s="2"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I25" t="s">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="7"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I25" s="7"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I26" s="7"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M27" s="2"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M28" s="2"/>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
         <v>45</v>
       </c>
-      <c r="M25">
+      <c r="M30">
         <f>120*10^6</f>
         <v>120000000</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I26" t="s">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
         <v>46</v>
       </c>
-      <c r="M26">
-        <f>M25/10^6</f>
+      <c r="M31">
+        <f>M30/10^6</f>
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N29" s="1"/>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
After experiments for min_xt
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>Version</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Measurement of task switch time</t>
+  </si>
+  <si>
+    <t>2nd board</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -543,7 +546,6 @@
     <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="8" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
@@ -1282,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O34"/>
+  <dimension ref="B1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,12 +1305,12 @@
     <col min="15" max="15" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1332,8 +1334,11 @@
       </c>
       <c r="N3" s="19"/>
       <c r="O3" s="20"/>
-    </row>
-    <row r="4" spans="2:15" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1366,8 +1371,17 @@
       <c r="O4" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>47</v>
       </c>
@@ -1397,11 +1411,11 @@
         <v>2.154559478768971</v>
       </c>
       <c r="O5" s="2">
-        <f>N5*$M$31</f>
+        <f>N5*$M$33</f>
         <v>258.5471374522765</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>47</v>
       </c>
@@ -1431,11 +1445,11 @@
         <v>1.0532968190436065</v>
       </c>
       <c r="O6" s="22">
-        <f>N6*$M$31</f>
+        <f>N6*$M$33</f>
         <v>126.39561828523279</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>31</v>
       </c>
@@ -1465,11 +1479,11 @@
         <v>6.0566417133028079</v>
       </c>
       <c r="O7" s="2">
-        <f>N7*$M$31</f>
+        <f>N7*$M$33</f>
         <v>726.79700559633693</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>31</v>
       </c>
@@ -1499,11 +1513,11 @@
         <v>1.1491082919654347</v>
       </c>
       <c r="O8" s="23">
-        <f>N8*$M$31</f>
+        <f>N8*$M$33</f>
         <v>137.89299503585218</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1536,11 +1550,11 @@
         <v>7.3253633380215657</v>
       </c>
       <c r="O9" s="21">
-        <f t="shared" ref="O9:O11" si="1">N9*$M$31</f>
+        <f t="shared" ref="O9:O14" si="1">N9*$M$33</f>
         <v>879.04360056258793</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1591,7 @@
         <v>976.68967313452265</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -1614,7 +1628,7 @@
         <v>1131.7765118647903</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>47</v>
       </c>
@@ -1636,11 +1650,25 @@
       <c r="I12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="24"/>
-    </row>
-    <row r="13" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="2"/>
+      <c r="N12" s="24">
+        <f>1.61/2</f>
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="O12" s="22">
+        <f t="shared" si="1"/>
+        <v>96.600000000000009</v>
+      </c>
+      <c r="R12" s="24">
+        <f>1.61/2</f>
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="S12" s="22">
+        <f t="shared" ref="S12:S14" si="2">R12*$M$33</f>
+        <v>96.600000000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -1662,11 +1690,25 @@
       <c r="I13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="24"/>
-    </row>
-    <row r="14" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="2"/>
+      <c r="N13" s="24">
+        <f>1.8/2</f>
+        <v>0.9</v>
+      </c>
+      <c r="O13" s="23">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="R13" s="24">
+        <f>1.8/2</f>
+        <v>0.9</v>
+      </c>
+      <c r="S13" s="23">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -1691,11 +1733,25 @@
       <c r="I14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="24"/>
-    </row>
-    <row r="15" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="2"/>
+      <c r="N14" s="24">
+        <f>13.84/2</f>
+        <v>6.92</v>
+      </c>
+      <c r="O14" s="21">
+        <f t="shared" si="1"/>
+        <v>830.4</v>
+      </c>
+      <c r="R14" s="24">
+        <f>13.87/2</f>
+        <v>6.9349999999999996</v>
+      </c>
+      <c r="S14" s="21">
+        <f t="shared" si="2"/>
+        <v>832.19999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -1726,11 +1782,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O15" s="2" t="e">
-        <f t="shared" ref="O15:O22" si="2">N15*$M$31</f>
+        <f>N15*$M$33</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -1761,11 +1817,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="2" t="e">
-        <f t="shared" si="2"/>
+        <f>N16*$M$33</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -1798,11 +1854,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O17" s="2" t="e">
-        <f t="shared" si="2"/>
+        <f>N17*$M$33</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -1833,11 +1889,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O18" s="2" t="e">
-        <f t="shared" si="2"/>
+        <f>N18*$M$33</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1870,11 +1926,11 @@
         <v>7.2296124927703875</v>
       </c>
       <c r="O19" s="21">
-        <f t="shared" si="2"/>
+        <f>N19*$M$33</f>
         <v>867.55349913244652</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -1891,7 +1947,7 @@
         <v>2</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -1900,18 +1956,18 @@
         <v>40</v>
       </c>
       <c r="M20" s="2">
-        <v>122144</v>
+        <v>138320</v>
       </c>
       <c r="N20" s="1">
         <f t="shared" ref="N20" si="3">10^6/M20</f>
-        <v>8.1870578988734604</v>
-      </c>
-      <c r="O20" s="2">
-        <f t="shared" si="2"/>
-        <v>982.44694786481523</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7.2296124927703875</v>
+      </c>
+      <c r="O20" s="21">
+        <f>N20*$M$33</f>
+        <v>867.55349913244652</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1984,7 @@
         <v>2</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -1937,18 +1993,18 @@
         <v>40</v>
       </c>
       <c r="M21" s="2">
-        <v>108784</v>
+        <v>122144</v>
       </c>
       <c r="N21" s="1">
         <f t="shared" ref="N21" si="4">10^6/M21</f>
-        <v>9.1925283129872035</v>
+        <v>8.1870578988734604</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="2"/>
-        <v>1103.1033975584644</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f>N21*$M$33</f>
+        <v>982.44694786481523</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>5</v>
       </c>
@@ -1965,69 +2021,147 @@
         <v>2</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="24"/>
-    </row>
-    <row r="23" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="7"/>
+      <c r="M22" s="2">
+        <v>108784</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" ref="N22" si="5">10^6/M22</f>
+        <v>9.1925283129872035</v>
+      </c>
+      <c r="O22" s="2">
+        <f>N22*$M$33</f>
+        <v>1103.1033975584644</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="M23" s="2"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I24" s="7"/>
+    <row r="24" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="M24" s="2"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N24" s="24">
+        <f>12.99/2</f>
+        <v>6.4950000000000001</v>
+      </c>
+      <c r="O24" s="21">
+        <f>N24*$M$33</f>
+        <v>779.4</v>
+      </c>
+      <c r="R24" s="24">
+        <v>6.51</v>
+      </c>
+      <c r="S24" s="21">
+        <f t="shared" ref="S24" si="6">R24*$M$33</f>
+        <v>781.19999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I25" s="7"/>
       <c r="M25" s="2"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I26" s="7"/>
       <c r="M26" s="2"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I27" s="7"/>
       <c r="M27" s="2"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I28" s="7"/>
       <c r="M28" s="2"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I30" t="s">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M29" s="2"/>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M30" s="2"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
         <v>45</v>
       </c>
-      <c r="M30">
+      <c r="M32">
         <f>120*10^6</f>
         <v>120000000</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I31" t="s">
+    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
         <v>46</v>
       </c>
-      <c r="M31">
-        <f>M30/10^6</f>
+      <c r="M33">
+        <f>M32/10^6</f>
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N34" s="1"/>
+    <row r="35" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="N36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Optimisations for await_xt and fix build flags
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
   <si>
     <t>Version</t>
   </si>
@@ -186,12 +186,6 @@
     <t>Clock speed</t>
   </si>
   <si>
-    <t>Ops per us</t>
-  </si>
-  <si>
-    <t>k22ptmin_loop_only</t>
-  </si>
-  <si>
     <t>Mean ops per task</t>
   </si>
   <si>
@@ -199,6 +193,48 @@
   </si>
   <si>
     <t>2nd board</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>DebugLLVM_NS</t>
+  </si>
+  <si>
+    <t>#define LOOP_ONLY in main.c</t>
+  </si>
+  <si>
+    <t>DebugLLVM</t>
+  </si>
+  <si>
+    <t>k22ptmin_xt</t>
+  </si>
+  <si>
+    <t>k22awaitmin_xt</t>
+  </si>
+  <si>
+    <t>Build configuration</t>
+  </si>
+  <si>
+    <t>Special build</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>#define UNUSED_TASK_COUNT 2 in main_cpp.cpp</t>
+  </si>
+  <si>
+    <t>#define UNUSED_TASK_COUNT 2 in ptmain_cpp.cpp</t>
+  </si>
+  <si>
+    <t>#define UNUSED_TASK_COUNT 1 in ptmain_cpp.cpp</t>
+  </si>
+  <si>
+    <t>#define UNUSED_TASK_COUNT 1 in main_cpp.cpp</t>
+  </si>
+  <si>
+    <t>Ops per µs</t>
   </si>
 </sst>
 </file>
@@ -493,7 +529,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -502,7 +538,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -510,6 +545,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,9 +573,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,10 +582,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="9" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="7" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="8" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
@@ -1284,891 +1319,933 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S36"/>
+  <dimension ref="B1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="12" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="12" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="2:21" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="3" spans="2:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="O3" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="23"/>
+      <c r="S3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="2:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="M3" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="20"/>
-      <c r="Q3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="O4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="2:19" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="M4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
+      <c r="D5" t="s">
+        <v>51</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>464132</v>
       </c>
-      <c r="N5" s="1">
-        <f>10^6/M5</f>
+      <c r="P5" s="1">
+        <f>10^6/O5</f>
         <v>2.154559478768971</v>
       </c>
-      <c r="O5" s="2">
-        <f>N5*$M$33</f>
+      <c r="Q5" s="2">
+        <f>P5*$O$31</f>
         <v>258.5471374522765</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>949400</v>
       </c>
-      <c r="N6" s="1">
-        <f>10^6/M6</f>
+      <c r="P6" s="1">
+        <f>10^6/O6</f>
         <v>1.0532968190436065</v>
       </c>
-      <c r="O6" s="22">
-        <f>N6*$M$33</f>
+      <c r="Q6" s="11">
+        <f>P6*$O$31</f>
         <v>126.39561828523279</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>165108</v>
       </c>
-      <c r="N7" s="1">
-        <f t="shared" ref="N7:N19" si="0">10^6/M7</f>
+      <c r="P7" s="1">
+        <f t="shared" ref="P7:P11" si="0">10^6/O7</f>
         <v>6.0566417133028079</v>
       </c>
-      <c r="O7" s="2">
-        <f>N7*$M$33</f>
+      <c r="Q7" s="2">
+        <f>P7*$O$31</f>
         <v>726.79700559633693</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>870240</v>
       </c>
-      <c r="N8" s="1">
+      <c r="P8" s="1">
         <f t="shared" si="0"/>
         <v>1.1491082919654347</v>
       </c>
-      <c r="O8" s="23">
-        <f>N8*$M$33</f>
+      <c r="Q8" s="12">
+        <f>P8*$O$31</f>
         <v>137.89299503585218</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
+      <c r="C9" t="s">
+        <v>52</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>136512</v>
       </c>
-      <c r="N9" s="1">
+      <c r="P9" s="1">
         <f t="shared" si="0"/>
         <v>7.3253633380215657</v>
       </c>
-      <c r="O9" s="21">
-        <f t="shared" ref="O9:O14" si="1">N9*$M$33</f>
+      <c r="Q9" s="10">
+        <f>P9*$O$31</f>
         <v>879.04360056258793</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>122864</v>
       </c>
-      <c r="N10" s="1">
+      <c r="P10" s="1">
         <f t="shared" si="0"/>
         <v>8.1390806094543553</v>
       </c>
-      <c r="O10" s="2">
-        <f t="shared" si="1"/>
+      <c r="Q10" s="2">
+        <f>P10*$O$31</f>
         <v>976.68967313452265</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>2</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>2</v>
       </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>106028</v>
       </c>
-      <c r="N11" s="1">
+      <c r="P11" s="1">
         <f t="shared" si="0"/>
         <v>9.4314709322065866</v>
       </c>
-      <c r="O11" s="2">
-        <f t="shared" si="1"/>
+      <c r="Q11" s="2">
+        <f>P11*$O$31</f>
         <v>1131.7765118647903</v>
       </c>
     </row>
-    <row r="12" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>2</v>
       </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="24">
+      <c r="O12" s="2"/>
+      <c r="P12" s="13">
         <f>1.61/2</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="O12" s="22">
-        <f t="shared" si="1"/>
+      <c r="Q12" s="11">
+        <f>P12*$O$31</f>
         <v>96.600000000000009</v>
       </c>
-      <c r="R12" s="24">
+      <c r="T12" s="13">
         <f>1.61/2</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="S12" s="22">
-        <f t="shared" ref="S12:S14" si="2">R12*$M$33</f>
+      <c r="U12" s="11">
+        <f>T12*$O$31</f>
         <v>96.600000000000009</v>
       </c>
     </row>
-    <row r="13" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="7" t="s">
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="24">
+      <c r="O13" s="2"/>
+      <c r="P13" s="13">
         <f>1.8/2</f>
         <v>0.9</v>
       </c>
-      <c r="O13" s="23">
-        <f t="shared" si="1"/>
+      <c r="Q13" s="12">
+        <f>P13*$O$31</f>
         <v>108</v>
       </c>
-      <c r="R13" s="24">
+      <c r="T13" s="13">
         <f>1.8/2</f>
         <v>0.9</v>
       </c>
-      <c r="S13" s="23">
-        <f t="shared" si="2"/>
+      <c r="U13" s="12">
+        <f>T13*$O$31</f>
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>2</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="24">
+      <c r="O14" s="2"/>
+      <c r="P14" s="13">
         <f>13.84/2</f>
         <v>6.92</v>
       </c>
-      <c r="O14" s="21">
-        <f t="shared" si="1"/>
+      <c r="Q14" s="10">
+        <f>P14*$O$31</f>
         <v>830.4</v>
       </c>
-      <c r="R14" s="24">
+      <c r="T14" s="13">
         <f>13.87/2</f>
         <v>6.9349999999999996</v>
       </c>
-      <c r="S14" s="21">
-        <f t="shared" si="2"/>
+      <c r="U14" s="10">
+        <f>T14*$O$31</f>
         <v>832.19999999999993</v>
       </c>
     </row>
-    <row r="15" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
+      <c r="C15" t="s">
+        <v>50</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="2" t="e">
-        <f>N15*$M$33</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O15" s="2">
+        <v>50093</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" ref="P15" si="1">10^6/O15</f>
+        <v>19.962869063541813</v>
+      </c>
+      <c r="Q15" s="2">
+        <f>P15*$O$31</f>
+        <v>2395.5442876250177</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
+      <c r="C16" t="s">
+        <v>50</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="2" t="e">
-        <f>N16*$M$33</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" s="2">
+        <v>357046</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" ref="P16" si="2">10^6/O16</f>
+        <v>2.8007595659942979</v>
+      </c>
+      <c r="Q16" s="12">
+        <f>P16*$O$31</f>
+        <v>336.09114791931574</v>
+      </c>
+      <c r="S16">
+        <v>409556</v>
+      </c>
+      <c r="T16" s="1">
+        <f t="shared" ref="T16" si="3">10^6/S16</f>
+        <v>2.4416685386125461</v>
+      </c>
+      <c r="U16" s="12">
+        <f>T16*$O$31</f>
+        <v>293.00022463350552</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
+      <c r="C17" t="s">
+        <v>52</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="2" t="e">
-        <f>N17*$M$33</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" s="2">
+        <v>138320</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" ref="P17" si="4">10^6/O17</f>
+        <v>7.2296124927703875</v>
+      </c>
+      <c r="Q17" s="10">
+        <f>P17*$O$31</f>
+        <v>867.55349913244652</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>2</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="2" t="e">
-        <f>N18*$M$33</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O18" s="2">
+        <v>122144</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" ref="P18" si="5">10^6/O18</f>
+        <v>8.1870578988734604</v>
+      </c>
+      <c r="Q18" s="2">
+        <f>P18*$O$31</f>
+        <v>982.44694786481523</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>2</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M19" s="2">
-        <v>138320</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" si="0"/>
-        <v>7.2296124927703875</v>
-      </c>
-      <c r="O19" s="21">
-        <f>N19*$M$33</f>
-        <v>867.55349913244652</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O19" s="2">
+        <v>108784</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" ref="P19" si="6">10^6/O19</f>
+        <v>9.1925283129872035</v>
+      </c>
+      <c r="Q19" s="2">
+        <f>P19*$O$31</f>
+        <v>1103.1033975584644</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>2</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="1"/>
+      <c r="T20" s="1">
+        <f>39/2</f>
+        <v>19.5</v>
+      </c>
+      <c r="U20" s="2">
+        <f>T20*$O$31</f>
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M20" s="2">
-        <v>138320</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" ref="N20" si="3">10^6/M20</f>
-        <v>7.2296124927703875</v>
-      </c>
-      <c r="O20" s="21">
-        <f>N20*$M$33</f>
-        <v>867.55349913244652</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21">
+      <c r="O21" s="2"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="12"/>
+      <c r="T21" s="13">
+        <f>3.99/2</f>
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="U21" s="12">
+        <f>T21*$O$31</f>
+        <v>239.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>2</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M21" s="2">
-        <v>122144</v>
-      </c>
-      <c r="N21" s="1">
-        <f t="shared" ref="N21" si="4">10^6/M21</f>
-        <v>8.1870578988734604</v>
-      </c>
-      <c r="O21" s="2">
-        <f>N21*$M$33</f>
-        <v>982.44694786481523</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M22" s="2">
-        <v>108784</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" ref="N22" si="5">10^6/M22</f>
-        <v>9.1925283129872035</v>
-      </c>
-      <c r="O22" s="2">
-        <f>N22*$M$33</f>
-        <v>1103.1033975584644</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="24">
+      <c r="O22" s="2"/>
+      <c r="P22" s="13">
         <f>12.99/2</f>
         <v>6.4950000000000001</v>
       </c>
-      <c r="O24" s="21">
-        <f>N24*$M$33</f>
+      <c r="Q22" s="10">
+        <f>P22*$O$31</f>
         <v>779.4</v>
       </c>
-      <c r="R24" s="24">
+      <c r="T22" s="13">
         <v>6.51</v>
       </c>
-      <c r="S24" s="21">
-        <f t="shared" ref="S24" si="6">R24*$M$33</f>
+      <c r="U22" s="10">
+        <f t="shared" ref="U22" si="7">T22*$O$31</f>
         <v>781.19999999999993</v>
       </c>
     </row>
-    <row r="25" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I25" s="7"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I26" s="7"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I27" s="7"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I28" s="7"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="M29" s="2"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="M30" s="2"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I32" t="s">
+    <row r="23" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="6"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K24" s="6"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K25" s="6"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K26" s="6"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O27" s="2"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O28" s="2"/>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
         <v>45</v>
       </c>
-      <c r="M32">
+      <c r="O30">
         <f>120*10^6</f>
         <v>120000000</v>
       </c>
     </row>
-    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" t="s">
-        <v>46</v>
-      </c>
-      <c r="M33">
-        <f>M32/10^6</f>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>62</v>
+      </c>
+      <c r="O31">
+        <f>O30/10^6</f>
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="N36" s="1"/>
+    <row r="33" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P34" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="5">
+    <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed clock speed for S/W timed projects. Added freertos base project
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Switch test (1)" sheetId="2" r:id="rId2"/>
+    <sheet name="Switch test (2)" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,8 +27,76 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bruce Belson</author>
+  </authors>
+  <commentList>
+    <comment ref="D24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bruce Belson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This setting controls the existence and per-cycle increment of a global counter, __co_g_cycles, which is excluded by the H/W counter version. This may have been the cause of a ~20% performance difference between H/W and S/W counter versions.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bruce Belson</author>
+  </authors>
+  <commentList>
+    <comment ref="D24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bruce Belson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This setting controls the existence and per-cycle increment of a global counter, __co_g_cycles, which is excluded by the H/W counter version. This may have been the cause of a ~20% performance difference between H/W and S/W counter versions.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="90">
   <si>
     <t>Version</t>
   </si>
@@ -236,12 +307,135 @@
   <si>
     <t>Ops per µs</t>
   </si>
+  <si>
+    <t>Sizes</t>
+  </si>
+  <si>
+    <t>Protothreads</t>
+  </si>
+  <si>
+    <t>Coroutines</t>
+  </si>
+  <si>
+    <r>
+      <t>Time per task (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Cycles per task</t>
+  </si>
+  <si>
+    <t>Underlying operation</t>
+  </si>
+  <si>
+    <t>Switching cost</t>
+  </si>
+  <si>
+    <t>Overall timing</t>
+  </si>
+  <si>
+    <r>
+      <t>Time (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    hex</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   19f8</t>
+  </si>
+  <si>
+    <t>k22awaitmin_xt.elf</t>
+  </si>
+  <si>
+    <t>k22ptmin_xt.elf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1d88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   11ac</t>
+  </si>
+  <si>
+    <t>1458</t>
+  </si>
+  <si>
+    <t>#define SET_GLOBAL_COUNTER</t>
+  </si>
+  <si>
+    <t>Clock speed:</t>
+  </si>
+  <si>
+    <t>21 MHz</t>
+  </si>
+  <si>
+    <t>120 MHz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +485,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -529,7 +736,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -552,6 +759,9 @@
     <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,6 +791,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1318,17 +1531,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
@@ -1342,136 +1555,126 @@
     <col min="17" max="17" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:28" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="3" spans="2:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+    <row r="2" spans="2:28" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="4" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="14" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19" t="s">
+      <c r="I4" s="19"/>
+      <c r="J4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="20"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="O3" s="21" t="s">
+      <c r="K4" s="21"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="O4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="23"/>
-      <c r="S3" t="s">
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
+      <c r="S4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="2:21" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="W4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="O4" s="5" t="s">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="O5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="U5" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="O5">
-        <v>464132</v>
-      </c>
-      <c r="P5" s="1">
-        <f>10^6/O5</f>
-        <v>2.154559478768971</v>
-      </c>
-      <c r="Q5" s="2">
-        <f>P5*$O$31</f>
-        <v>258.5471374522765</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W5" t="s">
+        <v>73</v>
+      </c>
+      <c r="X5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1497,27 +1700,30 @@
         <v>1</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="O6">
-        <v>949400</v>
+        <v>464132</v>
       </c>
       <c r="P6" s="1">
         <f>10^6/O6</f>
-        <v>1.0532968190436065</v>
-      </c>
-      <c r="Q6" s="11">
-        <f>P6*$O$31</f>
-        <v>126.39561828523279</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+        <v>2.154559478768971</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" ref="Q6:Q20" si="0">P6*$O$32</f>
+        <v>45.245749054148391</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
       </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
@@ -1525,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1534,21 +1740,21 @@
         <v>1</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O7">
-        <v>165108</v>
+        <v>949400</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" ref="P7:P11" si="0">10^6/O7</f>
-        <v>6.0566417133028079</v>
-      </c>
-      <c r="Q7" s="2">
-        <f>P7*$O$31</f>
-        <v>726.79700559633693</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+        <f>10^6/O7</f>
+        <v>1.0532968190436065</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="0"/>
+        <v>22.119233199915737</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -1571,41 +1777,38 @@
         <v>1</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="O8">
-        <v>870240</v>
+        <v>165108</v>
       </c>
       <c r="P8" s="1">
+        <f t="shared" ref="P8:P12" si="1">10^6/O8</f>
+        <v>6.0566417133028079</v>
+      </c>
+      <c r="Q8" s="2">
         <f t="shared" si="0"/>
-        <v>1.1491082919654347</v>
-      </c>
-      <c r="Q8" s="12">
-        <f>P8*$O$31</f>
-        <v>137.89299503585218</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+        <v>127.18947597935896</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
       <c r="H9">
         <v>2</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -1614,27 +1817,24 @@
         <v>40</v>
       </c>
       <c r="O9">
-        <v>136512</v>
+        <v>870240</v>
       </c>
       <c r="P9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1491082919654347</v>
+      </c>
+      <c r="Q9" s="12">
         <f t="shared" si="0"/>
-        <v>7.3253633380215657</v>
-      </c>
-      <c r="Q9" s="10">
-        <f>P9*$O$31</f>
-        <v>879.04360056258793</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+        <v>24.131274131274129</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
@@ -1648,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -1657,18 +1857,18 @@
         <v>40</v>
       </c>
       <c r="O10">
-        <v>122864</v>
+        <v>136512</v>
       </c>
       <c r="P10" s="1">
+        <f t="shared" si="1"/>
+        <v>7.3253633380215657</v>
+      </c>
+      <c r="Q10" s="10">
         <f t="shared" si="0"/>
-        <v>8.1390806094543553</v>
-      </c>
-      <c r="Q10" s="2">
-        <f>P10*$O$31</f>
-        <v>976.68967313452265</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>153.83263009845288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -1676,7 +1876,7 @@
         <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1691,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -1700,193 +1900,232 @@
         <v>40</v>
       </c>
       <c r="O11">
-        <v>106028</v>
+        <v>122864</v>
       </c>
       <c r="P11" s="1">
+        <f t="shared" si="1"/>
+        <v>8.1390806094543553</v>
+      </c>
+      <c r="Q11" s="2">
         <f t="shared" si="0"/>
-        <v>9.4314709322065866</v>
-      </c>
-      <c r="Q11" s="2">
-        <f>P11*$O$31</f>
-        <v>1131.7765118647903</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>170.92069279854147</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
       <c r="J12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="13">
+      <c r="O12">
+        <v>106028</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4314709322065866</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="0"/>
+        <v>198.06088957633833</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="13">
         <f>1.61/2</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="Q12" s="11">
-        <f>P12*$O$31</f>
-        <v>96.600000000000009</v>
-      </c>
-      <c r="T12" s="13">
+      <c r="Q13" s="11">
+        <f t="shared" si="0"/>
+        <v>16.905000000000001</v>
+      </c>
+      <c r="T13" s="13">
         <f>1.61/2</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="U12" s="11">
-        <f>T12*$O$31</f>
-        <v>96.600000000000009</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="U13" s="11">
+        <f>T13*$O$32</f>
+        <v>16.905000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="6" t="s">
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="13">
+      <c r="O14" s="2"/>
+      <c r="P14" s="13">
         <f>1.8/2</f>
         <v>0.9</v>
       </c>
-      <c r="Q13" s="12">
-        <f>P13*$O$31</f>
-        <v>108</v>
-      </c>
-      <c r="T13" s="13">
+      <c r="Q14" s="12">
+        <f t="shared" si="0"/>
+        <v>18.900000000000002</v>
+      </c>
+      <c r="T14" s="13">
         <f>1.8/2</f>
         <v>0.9</v>
       </c>
-      <c r="U13" s="12">
-        <f>T13*$O$31</f>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="U14" s="12">
+        <f>T14*$O$32</f>
+        <v>18.900000000000002</v>
+      </c>
+      <c r="W14">
+        <v>3324</v>
+      </c>
+      <c r="X14">
+        <v>140</v>
+      </c>
+      <c r="Y14">
+        <v>1060</v>
+      </c>
+      <c r="Z14">
+        <v>4524</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>52</v>
       </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6" t="s">
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="13">
+      <c r="O15" s="2"/>
+      <c r="P15" s="13">
         <f>13.84/2</f>
         <v>6.92</v>
       </c>
-      <c r="Q14" s="10">
-        <f>P14*$O$31</f>
-        <v>830.4</v>
-      </c>
-      <c r="T14" s="13">
+      <c r="Q15" s="10">
+        <f t="shared" si="0"/>
+        <v>145.32</v>
+      </c>
+      <c r="T15" s="13">
         <f>13.87/2</f>
         <v>6.9349999999999996</v>
       </c>
-      <c r="U14" s="10">
-        <f>T14*$O$31</f>
-        <v>832.19999999999993</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15" s="2">
-        <v>50093</v>
-      </c>
-      <c r="P15" s="1">
-        <f t="shared" ref="P15" si="1">10^6/O15</f>
-        <v>19.962869063541813</v>
-      </c>
-      <c r="Q15" s="2">
-        <f>P15*$O$31</f>
-        <v>2395.5442876250177</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U15" s="10">
+        <f>T15*$O$32</f>
+        <v>145.63499999999999</v>
+      </c>
+      <c r="W15">
+        <v>3964</v>
+      </c>
+      <c r="X15">
+        <v>140</v>
+      </c>
+      <c r="Y15">
+        <v>1104</v>
+      </c>
+      <c r="Z15">
+        <v>5208</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -1912,43 +2151,32 @@
         <v>1</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="O16" s="2">
-        <v>357046</v>
+        <v>50093</v>
       </c>
       <c r="P16" s="1">
         <f t="shared" ref="P16" si="2">10^6/O16</f>
-        <v>2.8007595659942979</v>
-      </c>
-      <c r="Q16" s="12">
-        <f>P16*$O$31</f>
-        <v>336.09114791931574</v>
-      </c>
-      <c r="S16">
-        <v>409556</v>
-      </c>
-      <c r="T16" s="1">
-        <f t="shared" ref="T16" si="3">10^6/S16</f>
-        <v>2.4416685386125461</v>
-      </c>
-      <c r="U16" s="12">
-        <f>T16*$O$31</f>
-        <v>293.00022463350552</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+        <v>19.962869063541813</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="0"/>
+        <v>419.22025033437808</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -1966,27 +2194,35 @@
         <v>40</v>
       </c>
       <c r="O17" s="2">
-        <v>138320</v>
+        <v>357046</v>
       </c>
       <c r="P17" s="1">
-        <f t="shared" ref="P17" si="4">10^6/O17</f>
-        <v>7.2296124927703875</v>
-      </c>
-      <c r="Q17" s="10">
-        <f>P17*$O$31</f>
-        <v>867.55349913244652</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="P17" si="3">10^6/O17</f>
+        <v>2.8007595659942979</v>
+      </c>
+      <c r="Q17" s="12">
+        <f t="shared" si="0"/>
+        <v>58.815950885880255</v>
+      </c>
+      <c r="S17">
+        <v>409556</v>
+      </c>
+      <c r="T17" s="1">
+        <f t="shared" ref="T17" si="4">10^6/S17</f>
+        <v>2.4416685386125461</v>
+      </c>
+      <c r="U17" s="12">
+        <f>T17*$O$32</f>
+        <v>51.27503931086347</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
       <c r="E18" t="b">
         <v>1</v>
       </c>
@@ -2000,7 +2236,7 @@
         <v>2</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
@@ -2009,18 +2245,18 @@
         <v>40</v>
       </c>
       <c r="O18" s="2">
-        <v>122144</v>
+        <v>138320</v>
       </c>
       <c r="P18" s="1">
         <f t="shared" ref="P18" si="5">10^6/O18</f>
-        <v>8.1870578988734604</v>
-      </c>
-      <c r="Q18" s="2">
-        <f>P18*$O$31</f>
-        <v>982.44694786481523</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+        <v>7.2296124927703875</v>
+      </c>
+      <c r="Q18" s="10">
+        <f t="shared" si="0"/>
+        <v>151.82186234817814</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -2028,7 +2264,7 @@
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -2043,7 +2279,7 @@
         <v>2</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
@@ -2052,202 +2288,1691 @@
         <v>40</v>
       </c>
       <c r="O19" s="2">
-        <v>108784</v>
+        <v>122144</v>
       </c>
       <c r="P19" s="1">
         <f t="shared" ref="P19" si="6">10^6/O19</f>
+        <v>8.1870578988734604</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="0"/>
+        <v>171.92821587634268</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" s="2">
+        <v>108784</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" ref="P20" si="7">10^6/O20</f>
         <v>9.1925283129872035</v>
       </c>
-      <c r="Q19" s="2">
-        <f>P19*$O$31</f>
-        <v>1103.1033975584644</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="Q20" s="2">
+        <f t="shared" si="0"/>
+        <v>193.04309457273126</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" s="6" t="s">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O20" s="2"/>
-      <c r="P20" s="1"/>
-      <c r="T20" s="1">
+      <c r="O21" s="2"/>
+      <c r="P21" s="1"/>
+      <c r="T21" s="1">
         <f>39/2</f>
         <v>19.5</v>
       </c>
-      <c r="U20" s="2">
-        <f>T20*$O$31</f>
-        <v>2340</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="U21" s="2">
+        <f>T21*$O$32</f>
+        <v>409.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" s="6" t="s">
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O21" s="2"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="12"/>
-      <c r="T21" s="13">
+      <c r="O22" s="2"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="12"/>
+      <c r="T22" s="13">
         <f>3.99/2</f>
         <v>1.9950000000000001</v>
       </c>
-      <c r="U21" s="12">
-        <f>T21*$O$31</f>
-        <v>239.4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="U22" s="12">
+        <f>T22*$O$32</f>
+        <v>41.895000000000003</v>
+      </c>
+      <c r="W22">
+        <v>5212</v>
+      </c>
+      <c r="X22">
+        <v>148</v>
+      </c>
+      <c r="Y22">
+        <v>1288</v>
+      </c>
+      <c r="Z22">
+        <v>6648</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>54</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>52</v>
       </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" s="6" t="s">
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O22" s="2"/>
-      <c r="P22" s="13">
+      <c r="O23" s="2"/>
+      <c r="P23" s="13">
         <f>12.99/2</f>
         <v>6.4950000000000001</v>
       </c>
-      <c r="Q22" s="10">
-        <f>P22*$O$31</f>
-        <v>779.4</v>
-      </c>
-      <c r="T22" s="13">
+      <c r="Q23" s="10">
+        <f>P23*$O$32</f>
+        <v>136.39500000000001</v>
+      </c>
+      <c r="T23" s="13">
         <v>6.51</v>
       </c>
-      <c r="U22" s="10">
-        <f t="shared" ref="U22" si="7">T22*$O$31</f>
-        <v>781.19999999999993</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="6"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="1"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="K24" s="6"/>
+      <c r="U23" s="10">
+        <f t="shared" ref="U23" si="8">T23*$O$32</f>
+        <v>136.71</v>
+      </c>
+      <c r="W23">
+        <v>6080</v>
+      </c>
+      <c r="X23">
+        <v>148</v>
+      </c>
+      <c r="Y23">
+        <v>1332</v>
+      </c>
+      <c r="Z23">
+        <v>7560</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="O24" s="2"/>
       <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="T24" s="13">
+        <f>4.64/2</f>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U24" s="12">
+        <f>T24*$O$32</f>
+        <v>48.72</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="K25" s="6"/>
       <c r="O25" s="2"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="K26" s="6"/>
       <c r="O26" s="2"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K27" s="6"/>
       <c r="O27" s="2"/>
       <c r="P27" s="1"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <f>T23/T15</f>
+        <v>0.9387166546503245</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
       <c r="O28" s="2"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="K30" t="s">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="O29" s="2"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
         <v>45</v>
       </c>
-      <c r="O30">
-        <f>120*10^6</f>
-        <v>120000000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="K31" t="s">
+      <c r="O31">
+        <v>21000000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
         <v>62</v>
       </c>
-      <c r="O31">
-        <f>O30/10^6</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P33" s="1"/>
+      <c r="O32">
+        <f>O31/10^6</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="34" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P34" s="1"/>
     </row>
+    <row r="35" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P35" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AB35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="12" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:28" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="2:28" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="4" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="O4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
+      <c r="S4" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="O5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5" t="s">
+        <v>73</v>
+      </c>
+      <c r="X5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="1" t="e">
+        <f>10^6/O6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q6" s="2" t="e">
+        <f t="shared" ref="Q6:Q20" si="0">P6*$O$32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7">
+        <v>5690781</v>
+      </c>
+      <c r="P7" s="1">
+        <f>10^6/O7</f>
+        <v>0.17572280500690501</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="0"/>
+        <v>21.086736600828601</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="1" t="e">
+        <f t="shared" ref="P8:P12" si="1">10^6/O8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q8" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9">
+        <v>5196505</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19243703219760205</v>
+      </c>
+      <c r="Q9" s="12">
+        <f t="shared" si="0"/>
+        <v>23.092443863712248</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10">
+        <v>609794</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6398980639363456</v>
+      </c>
+      <c r="Q10" s="10">
+        <f t="shared" si="0"/>
+        <v>196.78776767236147</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q11" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q12" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="13"/>
+      <c r="U13" s="11">
+        <f>T13*$O$32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="13"/>
+      <c r="U14" s="12">
+        <f>T14*$O$32</f>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>3324</v>
+      </c>
+      <c r="X14">
+        <v>140</v>
+      </c>
+      <c r="Y14">
+        <v>1060</v>
+      </c>
+      <c r="Z14">
+        <v>4524</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="13"/>
+      <c r="U15" s="10">
+        <f>T15*$O$32</f>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>3964</v>
+      </c>
+      <c r="X15">
+        <v>140</v>
+      </c>
+      <c r="Y15">
+        <v>1104</v>
+      </c>
+      <c r="Z15">
+        <v>5208</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="1" t="e">
+        <f t="shared" ref="P16:P20" si="2">10^6/O16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q16" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" s="2">
+        <v>2388806</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.41861917627467449</v>
+      </c>
+      <c r="Q17" s="12">
+        <f t="shared" si="0"/>
+        <v>50.234301152960938</v>
+      </c>
+      <c r="R17" s="2">
+        <f>Q17-Q9</f>
+        <v>27.141857289248691</v>
+      </c>
+      <c r="T17" s="1" t="e">
+        <f t="shared" ref="T17" si="3">10^6/S17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U17" s="12" t="e">
+        <f>T17*$O$32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O18" s="2">
+        <v>538043</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8585875106636458</v>
+      </c>
+      <c r="Q18" s="10">
+        <f t="shared" si="0"/>
+        <v>223.03050127963749</v>
+      </c>
+      <c r="R18" s="2">
+        <f>Q18-Q10</f>
+        <v>26.242733607276023</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="2">
+        <f>T21*$O$32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="12"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="12">
+        <f>T22*$O$32</f>
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>5212</v>
+      </c>
+      <c r="X22">
+        <v>148</v>
+      </c>
+      <c r="Y22">
+        <v>1288</v>
+      </c>
+      <c r="Z22">
+        <v>6648</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="10">
+        <f>P23*$O$32</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="13"/>
+      <c r="U23" s="10">
+        <f t="shared" ref="U23" si="4">T23*$O$32</f>
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>6080</v>
+      </c>
+      <c r="X23">
+        <v>148</v>
+      </c>
+      <c r="Y23">
+        <v>1332</v>
+      </c>
+      <c r="Z23">
+        <v>7560</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="1"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="12">
+        <f>T24*$O$32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="6"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K26" s="6"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K27" s="6"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="1"/>
+      <c r="T27" t="e">
+        <f>T23/T15</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="O28" s="2"/>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="O29" s="2"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>45</v>
+      </c>
+      <c r="O31">
+        <v>120000000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>62</v>
+      </c>
+      <c r="O32">
+        <f>O31/10^6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="O4:Q4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>5212</v>
+      </c>
+      <c r="D5">
+        <v>148</v>
+      </c>
+      <c r="E5">
+        <v>1288</v>
+      </c>
+      <c r="F5">
+        <v>6648</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>6080</v>
+      </c>
+      <c r="D8">
+        <v>148</v>
+      </c>
+      <c r="E8">
+        <v>1332</v>
+      </c>
+      <c r="F8">
+        <v>7560</v>
+      </c>
+      <c r="G8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3324</v>
+      </c>
+      <c r="D11">
+        <v>140</v>
+      </c>
+      <c r="E11">
+        <v>1060</v>
+      </c>
+      <c r="F11">
+        <v>4524</v>
+      </c>
+      <c r="G11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>3964</v>
+      </c>
+      <c r="D14">
+        <v>140</v>
+      </c>
+      <c r="E14">
+        <v>1104</v>
+      </c>
+      <c r="F14">
+        <v>5208</v>
+      </c>
+      <c r="G14">
+        <v>1458</v>
+      </c>
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1">
+        <f>120*10^6</f>
+        <v>120000000</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <f>D1/10^6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1">
+        <f>1.61/2</f>
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="D7" s="2">
+        <f>C7*$D$2</f>
+        <v>96.600000000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="1">
+        <f>1.8/2</f>
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="2">
+        <f>C8*$D$2</f>
+        <v>108</v>
+      </c>
+      <c r="E8" s="1">
+        <f>C8-$C$7</f>
+        <v>9.4999999999999973E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <f>E8*$D$2</f>
+        <v>11.399999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1">
+        <f>3.99/2</f>
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <f>C9*$D$2</f>
+        <v>239.4</v>
+      </c>
+      <c r="E9" s="1">
+        <f>C9-$C$7</f>
+        <v>1.19</v>
+      </c>
+      <c r="F9" s="2">
+        <f>E9*$D$2</f>
+        <v>142.79999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1">
+        <f>1.8/2</f>
+        <v>0.9</v>
+      </c>
+      <c r="D13" s="2">
+        <f>C13*$D$2</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1">
+        <f>3.99/2</f>
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="D14" s="2">
+        <f>C14*$D$2</f>
+        <v>239.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
freertos2 - added S/W timer and set clock to 120 MHz
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -41,7 +41,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Bruce Belson:</t>
         </r>
@@ -50,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This setting controls the existence and per-cycle increment of a global counter, __co_g_cycles, which is excluded by the H/W counter version. This may have been the cause of a ~20% performance difference between H/W and S/W counter versions.</t>
@@ -75,7 +75,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Bruce Belson:</t>
         </r>
@@ -84,7 +84,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This setting controls the existence and per-cycle increment of a global counter, __co_g_cycles, which is excluded by the H/W counter version. This may have been the cause of a ~20% performance difference between H/W and S/W counter versions.</t>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="92">
   <si>
     <t>Version</t>
   </si>
@@ -429,6 +429,12 @@
   </si>
   <si>
     <t>120 MHz</t>
+  </si>
+  <si>
+    <t>freertos2</t>
+  </si>
+  <si>
+    <t>Debug</t>
   </si>
 </sst>
 </file>
@@ -490,14 +496,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -762,6 +768,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,9 +800,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1535,7 +1541,7 @@
   <dimension ref="B1:AB35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,37 +1572,37 @@
       <c r="B2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="15" t="s">
         <v>88</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="4" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="15" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20" t="s">
+      <c r="I4" s="20"/>
+      <c r="J4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="21"/>
+      <c r="K4" s="22"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="25"/>
       <c r="S4" t="s">
         <v>48</v>
       </c>
@@ -2612,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2644,37 +2650,37 @@
       <c r="B2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="15" t="s">
         <v>89</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="4" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="15" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20" t="s">
+      <c r="I4" s="20"/>
+      <c r="J4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="21"/>
+      <c r="K4" s="22"/>
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="25"/>
       <c r="S4" t="s">
         <v>48</v>
       </c>
@@ -3578,14 +3584,84 @@
       </c>
     </row>
     <row r="25" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K25" s="6"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="1"/>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O25" s="2">
+        <v>203100</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" ref="P25" si="5">10^6/O25</f>
+        <v>4.9236829148202856</v>
+      </c>
+      <c r="Q25" s="2">
+        <f t="shared" ref="Q25" si="6">P25*$O$32</f>
+        <v>590.84194977843424</v>
+      </c>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="K26" s="6"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="1"/>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O26" s="2">
+        <v>333998</v>
+      </c>
+      <c r="P26" s="1">
+        <f t="shared" ref="P26" si="7">10^6/O26</f>
+        <v>2.9940299043706848</v>
+      </c>
+      <c r="Q26" s="2">
+        <f t="shared" ref="Q26" si="8">P26*$O$32</f>
+        <v>359.28358852448218</v>
+      </c>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
       <c r="K27" s="6"/>

</xml_diff>

<commit_message>
Completed context switch projects
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -19,6 +19,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Switch test (2)'!$A$5:$AA$32</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -97,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="125">
   <si>
     <t>Version</t>
   </si>
@@ -497,6 +500,45 @@
   <si>
     <t>Program size (bytes)</t>
   </si>
+  <si>
+    <t>mqxmin_xt</t>
+  </si>
+  <si>
+    <t>DebugLLVM_LoopOnly</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>freertos2_xt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   18c4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2b60</t>
+  </si>
+  <si>
+    <t>freertos2_xt.elf</t>
+  </si>
+  <si>
+    <t>mqxmin_xt.elf</t>
+  </si>
+  <si>
+    <t>Results (board 1)</t>
+  </si>
+  <si>
+    <t>Results (board 2)</t>
+  </si>
+  <si>
+    <t>Switching cost (board 1)</t>
+  </si>
+  <si>
+    <t>Switching cost (board 2)</t>
+  </si>
+  <si>
+    <t>Time for context switch</t>
+  </si>
 </sst>
 </file>
 
@@ -505,7 +547,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,6 +616,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -803,7 +853,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -814,8 +864,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -838,12 +889,15 @@
     <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -874,20 +928,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="8" builtinId="34"/>
     <cellStyle name="20% - Accent4" xfId="9" builtinId="42"/>
+    <cellStyle name="Calculation" xfId="10" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,10 +1083,10 @@
                   <c:v>Coroutines</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MQX Lite</c:v>
+                  <c:v>FreeRTOS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>FreeRTOS</c:v>
+                  <c:v>MQX Lite</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1040,16 +1098,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.671422719069704E-2</c:v>
+                  <c:v>1.7000000000000015E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24289637126776947</c:v>
+                  <c:v>0.20849999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7730597900987055</c:v>
+                  <c:v>2.5034999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8183070993637798</c:v>
+                  <c:v>2.8584999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1066,11 +1124,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="230607096"/>
-        <c:axId val="230609056"/>
+        <c:axId val="403756888"/>
+        <c:axId val="402671376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="230607096"/>
+        <c:axId val="403756888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1171,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230609056"/>
+        <c:crossAx val="402671376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1121,7 +1179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="230609056"/>
+        <c:axId val="402671376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230607096"/>
+        <c:crossAx val="403756888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1393,10 +1451,10 @@
                   <c:v>Coroutines</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MQX Lite</c:v>
+                  <c:v>FreeRTOS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>FreeRTOS</c:v>
+                  <c:v>MQX Lite</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1414,10 +1472,10 @@
                   <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>152</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1434,11 +1492,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="471474832"/>
-        <c:axId val="471472480"/>
+        <c:axId val="403901328"/>
+        <c:axId val="401764896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="471474832"/>
+        <c:axId val="403901328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,7 +1539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471472480"/>
+        <c:crossAx val="401764896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1489,7 +1547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471472480"/>
+        <c:axId val="401764896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471474832"/>
+        <c:crossAx val="403901328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1730,7 +1788,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1802,11 +1859,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="475056408"/>
-        <c:axId val="475050528"/>
+        <c:axId val="401765680"/>
+        <c:axId val="401766072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475056408"/>
+        <c:axId val="401765680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,7 +1906,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475050528"/>
+        <c:crossAx val="401766072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1857,7 +1914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="475050528"/>
+        <c:axId val="401766072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,7 +1960,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1964,7 +2020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475056408"/>
+        <c:crossAx val="401765680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2131,10 +2187,10 @@
                   <c:v>Coroutines</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MQX Lite</c:v>
+                  <c:v>FreeRTOS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>FreeRTOS</c:v>
+                  <c:v>MQX Lite</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2146,16 +2202,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.671422719069704E-2</c:v>
+                  <c:v>1.7000000000000015E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24289637126776947</c:v>
+                  <c:v>0.20849999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7730597900987055</c:v>
+                  <c:v>2.5034999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8183070993637798</c:v>
+                  <c:v>2.8584999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2172,11 +2228,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="475907008"/>
-        <c:axId val="466396744"/>
+        <c:axId val="401766856"/>
+        <c:axId val="401767248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475907008"/>
+        <c:axId val="401766856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2219,7 +2275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466396744"/>
+        <c:crossAx val="401767248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2227,7 +2283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="466396744"/>
+        <c:axId val="401767248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2334,7 +2390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475907008"/>
+        <c:crossAx val="401766856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2501,10 +2557,10 @@
                   <c:v>Coroutines</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MQX Lite</c:v>
+                  <c:v>FreeRTOS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>FreeRTOS</c:v>
+                  <c:v>MQX Lite</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2522,10 +2578,10 @@
                   <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>152</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2542,11 +2598,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="620468448"/>
-        <c:axId val="606213696"/>
+        <c:axId val="401769600"/>
+        <c:axId val="401769992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="620468448"/>
+        <c:axId val="401769600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2589,7 +2645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="606213696"/>
+        <c:crossAx val="401769992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2597,7 +2653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="606213696"/>
+        <c:axId val="401769992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2704,7 +2760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="620468448"/>
+        <c:crossAx val="401769600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5764,7 +5820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5794,37 +5852,37 @@
       <c r="B2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>88</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="4" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="16" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19" t="s">
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21" t="s">
+      <c r="I4" s="23"/>
+      <c r="J4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="22"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-      <c r="O4" s="23" t="s">
+      <c r="O4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="28"/>
       <c r="S4" t="s">
         <v>48</v>
       </c>
@@ -6842,85 +6900,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AE41"/>
+  <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:F44"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="12" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="28"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="21" width="12" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="2:31" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>89</v>
       </c>
       <c r="D2" s="8"/>
     </row>
-    <row r="4" spans="2:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="16" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21" t="s">
+      <c r="I4" s="36"/>
+      <c r="J4" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="O4" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25"/>
-      <c r="S4" t="s">
-        <v>69</v>
-      </c>
-      <c r="V4" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="K4" s="38"/>
+      <c r="L4" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="M4" s="30"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="R4" s="30"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="U4" s="39"/>
+      <c r="V4" s="40" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="2:31" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+    </row>
+    <row r="5" spans="1:27" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
@@ -6951,52 +7021,56 @@
       <c r="K5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="O5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="V5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="X5" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="V5" t="s">
         <v>73</v>
       </c>
+      <c r="W5" t="s">
+        <v>74</v>
+      </c>
+      <c r="X5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z5" s="17" t="s">
+        <v>77</v>
+      </c>
       <c r="AA5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD5" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -7024,16 +7098,16 @@
       <c r="K6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="26" t="e">
-        <f>10^6/O6</f>
+      <c r="M6" s="15" t="e">
+        <f>10^6/L6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q6" s="2" t="e">
-        <f t="shared" ref="Q6:Q20" si="0">P6*$O$38</f>
+      <c r="N6" s="2" t="e">
+        <f t="shared" ref="N6:N20" si="0">M6*$L$39</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -7061,19 +7135,19 @@
       <c r="K7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O7">
+      <c r="L7">
         <v>5690781</v>
       </c>
-      <c r="P7" s="26">
-        <f>10^6/O7</f>
+      <c r="M7" s="15">
+        <f>10^6/L7</f>
         <v>0.17572280500690501</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="N7" s="11">
         <f t="shared" si="0"/>
         <v>21.086736600828601</v>
       </c>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -7098,16 +7172,16 @@
       <c r="K8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="26" t="e">
-        <f t="shared" ref="P8:P12" si="1">10^6/O8</f>
+      <c r="M8" s="15" t="e">
+        <f t="shared" ref="M8:M12" si="1">10^6/L8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q8" s="2" t="e">
+      <c r="N8" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -7132,45 +7206,45 @@
       <c r="K9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O9">
+      <c r="L9">
         <v>5196505</v>
       </c>
-      <c r="P9" s="26">
+      <c r="M9" s="15">
         <f t="shared" si="1"/>
         <v>0.19243703219760205</v>
       </c>
-      <c r="Q9" s="12">
+      <c r="N9" s="12">
         <f t="shared" si="0"/>
         <v>23.092443863712248</v>
       </c>
-      <c r="S9" s="26">
-        <f>P9-P7</f>
+      <c r="O9" s="15">
+        <f>M9-M7</f>
         <v>1.671422719069704E-2</v>
       </c>
-      <c r="T9" s="2">
-        <f t="shared" ref="T9" si="2">S9*$O$38</f>
+      <c r="P9" s="2">
+        <f t="shared" ref="P9" si="2">O9*$L$39</f>
         <v>2.0057072628836448</v>
       </c>
-      <c r="Z9">
+      <c r="V9">
         <v>4384</v>
       </c>
-      <c r="AA9">
+      <c r="W9">
         <v>140</v>
       </c>
-      <c r="AB9">
+      <c r="X9">
         <v>1148</v>
       </c>
-      <c r="AC9">
+      <c r="Y9">
         <v>5672</v>
       </c>
-      <c r="AD9">
+      <c r="Z9" s="17">
         <v>1628</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AA9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -7198,37 +7272,37 @@
       <c r="K10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O10">
+      <c r="L10">
         <v>609794</v>
       </c>
-      <c r="P10" s="26">
+      <c r="M10" s="15">
         <f t="shared" si="1"/>
         <v>1.6398980639363456</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="N10" s="10">
         <f t="shared" si="0"/>
         <v>196.78776767236147</v>
       </c>
-      <c r="Z10">
+      <c r="V10">
         <v>5096</v>
       </c>
-      <c r="AA10">
+      <c r="W10">
         <v>140</v>
       </c>
-      <c r="AB10">
+      <c r="X10">
         <v>1192</v>
       </c>
-      <c r="AC10">
+      <c r="Y10">
         <v>6428</v>
       </c>
-      <c r="AD10" s="28" t="s">
+      <c r="Z10" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AA10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -7259,16 +7333,16 @@
       <c r="K11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="P11" s="26" t="e">
+      <c r="M11" s="15" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q11" s="2" t="e">
+      <c r="N11" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -7299,24 +7373,24 @@
       <c r="K12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="26" t="e">
+      <c r="M12" s="15" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q12" s="2" t="e">
+      <c r="N12" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="2:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="b">
+        <v>1</v>
+      </c>
       <c r="B13" t="s">
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -7336,19 +7410,46 @@
       <c r="K13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="11">
+      <c r="L13" s="2"/>
+      <c r="M13" s="16">
+        <f>0.283/2</f>
+        <v>0.14149999999999999</v>
+      </c>
+      <c r="N13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W13" s="13"/>
-      <c r="X13" s="11">
-        <f>W13*$O$38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16.979999999999997</v>
+      </c>
+      <c r="R13" s="16">
+        <f>0.283/2</f>
+        <v>0.14149999999999999</v>
+      </c>
+      <c r="S13" s="11">
+        <f>R13*$L$39</f>
+        <v>16.979999999999997</v>
+      </c>
+      <c r="V13">
+        <v>2960</v>
+      </c>
+      <c r="W13">
+        <v>140</v>
+      </c>
+      <c r="X13">
+        <v>1060</v>
+      </c>
+      <c r="Y13">
+        <v>4160</v>
+      </c>
+      <c r="Z13" s="17">
+        <v>1040</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="b">
+        <v>1</v>
+      </c>
       <c r="B14" t="s">
         <v>53</v>
       </c>
@@ -7373,37 +7474,59 @@
       <c r="K14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="12">
+      <c r="L14" s="2"/>
+      <c r="M14" s="16">
+        <f>0.317/2</f>
+        <v>0.1585</v>
+      </c>
+      <c r="N14" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W14" s="13"/>
-      <c r="X14" s="12">
-        <f>W14*$O$38</f>
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <v>3324</v>
-      </c>
-      <c r="AA14">
+        <v>19.02</v>
+      </c>
+      <c r="O14" s="15">
+        <f>M14-M$13</f>
+        <v>1.7000000000000015E-2</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" ref="P14" si="3">O14*$L$39</f>
+        <v>2.0400000000000018</v>
+      </c>
+      <c r="R14" s="13">
+        <f>0.317/2</f>
+        <v>0.1585</v>
+      </c>
+      <c r="S14" s="12">
+        <f>R14*$L$39</f>
+        <v>19.02</v>
+      </c>
+      <c r="T14" s="15">
+        <f>R14-R$13</f>
+        <v>1.7000000000000015E-2</v>
+      </c>
+      <c r="U14">
+        <f>T14*$L$39</f>
+        <v>2.0400000000000018</v>
+      </c>
+      <c r="V14">
+        <v>3012</v>
+      </c>
+      <c r="W14">
         <v>140</v>
       </c>
-      <c r="AB14">
+      <c r="X14">
         <v>1060</v>
       </c>
-      <c r="AC14">
-        <v>4524</v>
-      </c>
-      <c r="AD14" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE14" t="s">
+      <c r="Y14">
+        <v>4212</v>
+      </c>
+      <c r="Z14" s="17">
+        <v>1074</v>
+      </c>
+      <c r="AA14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="2:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>53</v>
       </c>
@@ -7431,37 +7554,37 @@
       <c r="K15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="10">
+      <c r="L15" s="2"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W15" s="13"/>
-      <c r="X15" s="10">
-        <f>W15*$O$38</f>
-        <v>0</v>
-      </c>
-      <c r="Z15">
+      <c r="R15" s="13"/>
+      <c r="S15" s="10">
+        <f>R15*$L$39</f>
+        <v>0</v>
+      </c>
+      <c r="V15">
         <v>3964</v>
       </c>
-      <c r="AA15">
+      <c r="W15">
         <v>140</v>
       </c>
-      <c r="AB15">
+      <c r="X15">
         <v>1104</v>
       </c>
-      <c r="AC15">
+      <c r="Y15">
         <v>5208</v>
       </c>
-      <c r="AD15" s="6" t="s">
+      <c r="Z15" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AA15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -7489,17 +7612,17 @@
       <c r="K16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="26" t="e">
-        <f t="shared" ref="P16:P20" si="3">10^6/O16</f>
+      <c r="L16" s="2"/>
+      <c r="M16" s="15" t="e">
+        <f t="shared" ref="M16:M20" si="4">10^6/L16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q16" s="2" t="e">
+      <c r="N16" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -7527,54 +7650,53 @@
       <c r="K17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O17" s="2">
+      <c r="L17" s="2">
         <v>2388806</v>
       </c>
-      <c r="P17" s="26">
-        <f t="shared" si="3"/>
+      <c r="M17" s="15">
+        <f t="shared" si="4"/>
         <v>0.41861917627467449</v>
       </c>
-      <c r="Q17" s="12">
+      <c r="N17" s="12">
         <f t="shared" si="0"/>
         <v>50.234301152960938</v>
       </c>
-      <c r="S17" s="26">
-        <f>P17-P$7</f>
+      <c r="O17" s="15">
+        <f>M17-M$7</f>
         <v>0.24289637126776947</v>
       </c>
-      <c r="T17" s="2">
-        <f t="shared" ref="T17:T18" si="4">S17*$O$38</f>
+      <c r="P17" s="2">
+        <f t="shared" ref="P17:P18" si="5">O17*$L$39</f>
         <v>29.147564552132337</v>
       </c>
-      <c r="U17" s="2"/>
-      <c r="W17" s="1" t="e">
-        <f>10^6/V17</f>
+      <c r="R17" s="1" t="e">
+        <f>10^6/Q17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="X17" s="12" t="e">
-        <f>W17*$O$38</f>
+      <c r="S17" s="12" t="e">
+        <f>R17*$L$39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z17">
+      <c r="V17">
         <v>6236</v>
       </c>
-      <c r="AA17">
+      <c r="W17">
         <v>148</v>
       </c>
-      <c r="AB17">
+      <c r="X17">
         <v>1356</v>
       </c>
-      <c r="AC17">
+      <c r="Y17">
         <v>7740</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="Z17" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AA17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -7602,28 +7724,27 @@
       <c r="K18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O18" s="2">
+      <c r="L18" s="2">
         <v>538043</v>
       </c>
-      <c r="P18" s="26">
-        <f t="shared" si="3"/>
+      <c r="M18" s="15">
+        <f t="shared" si="4"/>
         <v>1.8585875106636458</v>
       </c>
-      <c r="Q18" s="10">
+      <c r="N18" s="10">
         <f t="shared" si="0"/>
         <v>223.03050127963749</v>
       </c>
-      <c r="S18" s="26">
-        <f>P18-P10</f>
+      <c r="O18" s="15">
+        <f>M18-M10</f>
         <v>0.21868944672730017</v>
       </c>
-      <c r="T18" s="2">
-        <f t="shared" si="4"/>
+      <c r="P18" s="2">
+        <f t="shared" si="5"/>
         <v>26.242733607276023</v>
       </c>
-      <c r="U18" s="2"/>
-    </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -7654,17 +7775,17 @@
       <c r="K19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O19" s="2"/>
-      <c r="P19" s="26" t="e">
-        <f t="shared" si="3"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="15" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q19" s="2" t="e">
+      <c r="N19" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -7695,17 +7816,17 @@
       <c r="K20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O20" s="2"/>
-      <c r="P20" s="26" t="e">
-        <f t="shared" si="3"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="15" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q20" s="2" t="e">
+      <c r="N20" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>54</v>
       </c>
@@ -7733,15 +7854,18 @@
       <c r="K21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O21" s="2"/>
-      <c r="P21" s="26"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="2">
-        <f>W21*$O$38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="2"/>
+      <c r="M21" s="15"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="2">
+        <f>R21*$L$39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="b">
+        <v>1</v>
+      </c>
       <c r="B22" t="s">
         <v>54</v>
       </c>
@@ -7769,34 +7893,59 @@
       <c r="K22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O22" s="2"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="12"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="12">
-        <f>W22*$O$38</f>
-        <v>0</v>
-      </c>
-      <c r="Z22">
-        <v>5212</v>
-      </c>
-      <c r="AA22">
+      <c r="L22" s="2"/>
+      <c r="M22" s="16">
+        <f>0.7/2</f>
+        <v>0.35</v>
+      </c>
+      <c r="N22" s="12">
+        <f t="shared" ref="N22" si="6">M22*$L$39</f>
+        <v>42</v>
+      </c>
+      <c r="O22" s="15">
+        <f>M22-M$13</f>
+        <v>0.20849999999999999</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" ref="P22" si="7">O22*$L$39</f>
+        <v>25.02</v>
+      </c>
+      <c r="R22" s="13">
+        <f>0.7/2</f>
+        <v>0.35</v>
+      </c>
+      <c r="S22" s="12">
+        <f>R22*$L$39</f>
+        <v>42</v>
+      </c>
+      <c r="T22" s="15">
+        <f>R22-R$13</f>
+        <v>0.20849999999999999</v>
+      </c>
+      <c r="U22">
+        <f>T22*$L$39</f>
+        <v>25.02</v>
+      </c>
+      <c r="V22">
+        <v>4904</v>
+      </c>
+      <c r="W22">
         <v>148</v>
       </c>
-      <c r="AB22">
+      <c r="X22">
         <v>1288</v>
       </c>
-      <c r="AC22">
-        <v>6648</v>
-      </c>
-      <c r="AD22" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE22" t="s">
+      <c r="Y22">
+        <v>6340</v>
+      </c>
+      <c r="Z22" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA22" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -7824,37 +7973,37 @@
       <c r="K23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O23" s="2"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="10">
-        <f>P23*$O$38</f>
-        <v>0</v>
-      </c>
-      <c r="W23" s="13"/>
-      <c r="X23" s="10">
-        <f t="shared" ref="X23" si="5">W23*$O$38</f>
-        <v>0</v>
-      </c>
-      <c r="Z23">
+      <c r="L23" s="2"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="10">
+        <f>M23*$L$39</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="13"/>
+      <c r="S23" s="10">
+        <f t="shared" ref="S23" si="8">R23*$L$39</f>
+        <v>0</v>
+      </c>
+      <c r="V23">
         <v>6080</v>
       </c>
-      <c r="AA23">
+      <c r="W23">
         <v>148</v>
       </c>
-      <c r="AB23">
+      <c r="X23">
         <v>1332</v>
       </c>
-      <c r="AC23">
+      <c r="Y23">
         <v>7560</v>
       </c>
-      <c r="AD23" s="28" t="s">
+      <c r="Z23" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AE23" t="s">
+      <c r="AA23" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>54</v>
       </c>
@@ -7885,15 +8034,15 @@
       <c r="K24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O24" s="2"/>
-      <c r="P24" s="26"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="12">
-        <f>W24*$O$38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="2"/>
+      <c r="M24" s="15"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="12">
+        <f>R24*$L$39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>90</v>
       </c>
@@ -7921,19 +8070,19 @@
       <c r="K25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O25" s="2">
+      <c r="L25" s="2">
         <v>203100</v>
       </c>
-      <c r="P25" s="26">
-        <f t="shared" ref="P25" si="6">10^6/O25</f>
+      <c r="M25" s="15">
+        <f t="shared" ref="M25" si="9">10^6/L25</f>
         <v>4.9236829148202856</v>
       </c>
-      <c r="Q25" s="2">
-        <f t="shared" ref="Q25" si="7">P25*$O$38</f>
+      <c r="N25" s="2">
+        <f t="shared" ref="N25" si="10">M25*$L$39</f>
         <v>590.84194977843424</v>
       </c>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>90</v>
       </c>
@@ -7961,46 +8110,45 @@
       <c r="K26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="2">
+      <c r="L26" s="2">
         <v>333998</v>
       </c>
-      <c r="P26" s="26">
-        <f t="shared" ref="P26:P28" si="8">10^6/O26</f>
+      <c r="M26" s="15">
+        <f t="shared" ref="M26:M29" si="11">10^6/L26</f>
         <v>2.9940299043706848</v>
       </c>
-      <c r="Q26" s="2">
-        <f t="shared" ref="Q26:Q28" si="9">P26*$O$38</f>
+      <c r="N26" s="2">
+        <f t="shared" ref="N26:N29" si="12">M26*$L$39</f>
         <v>359.28358852448218</v>
       </c>
-      <c r="S26" s="26">
-        <f>P26-P7</f>
+      <c r="O26" s="15">
+        <f>M26-M7</f>
         <v>2.8183070993637798</v>
       </c>
-      <c r="T26" s="2">
-        <f t="shared" ref="T26:T30" si="10">S26*$O$38</f>
+      <c r="P26" s="2">
+        <f t="shared" ref="P26:P32" si="13">O26*$L$39</f>
         <v>338.19685192365358</v>
       </c>
-      <c r="U26" s="2"/>
-      <c r="Z26">
+      <c r="V26">
         <v>6768</v>
       </c>
-      <c r="AA26">
+      <c r="W26">
         <v>152</v>
       </c>
-      <c r="AB26">
+      <c r="X26">
         <v>4344</v>
       </c>
-      <c r="AC26">
+      <c r="Y26">
         <v>11264</v>
       </c>
-      <c r="AD26" s="28" t="s">
+      <c r="Z26" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="AE26" t="s">
+      <c r="AA26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>90</v>
       </c>
@@ -8028,51 +8176,53 @@
       <c r="K27" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O27" s="2">
+      <c r="L27" s="2">
         <v>340668</v>
       </c>
-      <c r="P27" s="26">
-        <f t="shared" ref="P27" si="11">10^6/O27</f>
+      <c r="M27" s="15">
+        <f t="shared" ref="M27" si="14">10^6/L27</f>
         <v>2.9354092547582984</v>
       </c>
-      <c r="Q27" s="2">
-        <f t="shared" ref="Q27" si="12">P27*$O$38</f>
+      <c r="N27" s="2">
+        <f t="shared" ref="N27:N28" si="15">M27*$L$39</f>
         <v>352.24911057099581</v>
       </c>
-      <c r="S27" s="26">
-        <f>P27-P7</f>
+      <c r="O27" s="15">
+        <f>M27-M7</f>
         <v>2.7596864497513933</v>
       </c>
-      <c r="T27" s="2">
-        <f t="shared" ref="T27" si="13">S27*$O$38</f>
+      <c r="P27" s="2">
+        <f t="shared" ref="P27:P28" si="16">O27*$L$39</f>
         <v>331.16237397016721</v>
       </c>
-      <c r="U27" s="2"/>
-      <c r="Z27">
+      <c r="V27">
         <v>7856</v>
       </c>
-      <c r="AA27">
+      <c r="W27">
         <v>144</v>
       </c>
-      <c r="AB27">
+      <c r="X27">
         <v>4344</v>
       </c>
-      <c r="AC27">
+      <c r="Y27">
         <v>12344</v>
       </c>
-      <c r="AD27">
+      <c r="Z27" s="17">
         <v>3038</v>
       </c>
-      <c r="AE27" t="s">
+      <c r="AA27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="b">
+        <v>1</v>
+      </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -8093,21 +8243,61 @@
         <v>1</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="O28" s="2">
-        <v>242656</v>
-      </c>
-      <c r="P28" s="26">
-        <f t="shared" si="8"/>
-        <v>4.121060266385336</v>
-      </c>
-      <c r="Q28" s="2">
-        <f t="shared" si="9"/>
-        <v>494.52723196624032</v>
-      </c>
-    </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="16">
+        <f>5.29/2</f>
+        <v>2.645</v>
+      </c>
+      <c r="N28" s="12">
+        <f t="shared" si="15"/>
+        <v>317.39999999999998</v>
+      </c>
+      <c r="O28" s="15">
+        <f>M28-M$13</f>
+        <v>2.5034999999999998</v>
+      </c>
+      <c r="P28" s="1">
+        <f t="shared" si="16"/>
+        <v>300.41999999999996</v>
+      </c>
+      <c r="R28" s="13">
+        <f>5.29/2</f>
+        <v>2.645</v>
+      </c>
+      <c r="S28" s="12">
+        <f>R28*$L$39</f>
+        <v>317.39999999999998</v>
+      </c>
+      <c r="T28" s="15">
+        <f>R28-R$13</f>
+        <v>2.5034999999999998</v>
+      </c>
+      <c r="U28">
+        <f>T28*$L$39</f>
+        <v>300.41999999999996</v>
+      </c>
+      <c r="V28">
+        <v>6676</v>
+      </c>
+      <c r="W28">
+        <v>144</v>
+      </c>
+      <c r="X28">
+        <v>4284</v>
+      </c>
+      <c r="Y28">
+        <v>11104</v>
+      </c>
+      <c r="Z28" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>92</v>
       </c>
@@ -8133,53 +8323,26 @@
         <v>1</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O29" s="2">
-        <v>339123</v>
-      </c>
-      <c r="P29" s="26">
-        <f t="shared" ref="P29" si="14">10^6/O29</f>
-        <v>2.9487825951056106</v>
-      </c>
-      <c r="Q29" s="2">
-        <f t="shared" ref="Q29" si="15">P29*$O$38</f>
-        <v>353.85391141267326</v>
-      </c>
-      <c r="S29" s="26">
-        <f>P29-P7</f>
-        <v>2.7730597900987055</v>
-      </c>
-      <c r="T29" s="2">
-        <f t="shared" si="10"/>
-        <v>332.76717481184465</v>
-      </c>
-      <c r="U29" s="2"/>
-      <c r="Z29">
-        <v>8644</v>
-      </c>
-      <c r="AA29">
-        <v>156</v>
-      </c>
-      <c r="AB29">
-        <v>4328</v>
-      </c>
-      <c r="AC29">
-        <v>13128</v>
-      </c>
-      <c r="AD29" s="28">
-        <v>3348</v>
-      </c>
-      <c r="AE29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="L29" s="2">
+        <v>242656</v>
+      </c>
+      <c r="M29" s="15">
+        <f t="shared" si="11"/>
+        <v>4.121060266385336</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="12"/>
+        <v>494.52723196624032</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -8202,95 +8365,234 @@
       <c r="K30" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O30" s="2">
+      <c r="L30" s="2">
+        <v>339123</v>
+      </c>
+      <c r="M30" s="15">
+        <f t="shared" ref="M30" si="17">10^6/L30</f>
+        <v>2.9487825951056106</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" ref="N30" si="18">M30*$L$39</f>
+        <v>353.85391141267326</v>
+      </c>
+      <c r="O30" s="15">
+        <f>M30-M7</f>
+        <v>2.7730597900987055</v>
+      </c>
+      <c r="P30" s="2">
+        <f t="shared" si="13"/>
+        <v>332.76717481184465</v>
+      </c>
+      <c r="V30">
+        <v>8644</v>
+      </c>
+      <c r="W30">
+        <v>156</v>
+      </c>
+      <c r="X30">
+        <v>4328</v>
+      </c>
+      <c r="Y30">
+        <v>13128</v>
+      </c>
+      <c r="Z30" s="17">
+        <v>3348</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L31" s="2">
         <v>324856</v>
       </c>
-      <c r="P30" s="26">
-        <f t="shared" ref="P30" si="16">10^6/O30</f>
+      <c r="M31" s="15">
+        <f t="shared" ref="M31" si="19">10^6/L31</f>
         <v>3.0782869948531042</v>
       </c>
-      <c r="Q30" s="2">
-        <f t="shared" ref="Q30" si="17">P30*$O$38</f>
+      <c r="N31" s="2">
+        <f t="shared" ref="N31" si="20">M31*$L$39</f>
         <v>369.39443938237252</v>
       </c>
-      <c r="S30" s="26">
-        <f>P30-P7</f>
+      <c r="O31" s="15">
+        <f>M31-M7</f>
         <v>2.9025641898461991</v>
       </c>
-      <c r="T30" s="2">
-        <f t="shared" si="10"/>
+      <c r="P31" s="2">
+        <f t="shared" si="13"/>
         <v>348.30770278154387</v>
       </c>
-      <c r="Z30">
+      <c r="V31">
         <v>11040</v>
       </c>
-      <c r="AA30">
+      <c r="W31">
         <v>156</v>
       </c>
-      <c r="AB30">
+      <c r="X31">
         <v>4332</v>
       </c>
-      <c r="AC30">
+      <c r="Y31">
         <v>15528</v>
       </c>
-      <c r="AD30" s="28" t="s">
+      <c r="Z31" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AA31" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="O31" s="2"/>
-      <c r="P31" s="1"/>
-    </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="O32" s="2"/>
-      <c r="P32" s="1"/>
-    </row>
-    <row r="33" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="O33" s="2"/>
-      <c r="P33" s="1"/>
-    </row>
-    <row r="34" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="O34" s="2"/>
-      <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="O35" s="2"/>
-      <c r="P35" s="1"/>
-    </row>
-    <row r="37" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K37" t="s">
+    <row r="32" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="16">
+        <f>6/2</f>
+        <v>3</v>
+      </c>
+      <c r="N32" s="10">
+        <f>M32*$L$39</f>
+        <v>360</v>
+      </c>
+      <c r="O32" s="15">
+        <f>M32-M$13</f>
+        <v>2.8584999999999998</v>
+      </c>
+      <c r="P32" s="1">
+        <f t="shared" si="13"/>
+        <v>343.02</v>
+      </c>
+      <c r="R32" s="16">
+        <f>6/2</f>
+        <v>3</v>
+      </c>
+      <c r="S32" s="12">
+        <f>R32*$L$39</f>
+        <v>360</v>
+      </c>
+      <c r="T32" s="15">
+        <f>R32-R$13</f>
+        <v>2.8584999999999998</v>
+      </c>
+      <c r="U32">
+        <f>T32*$L$39</f>
+        <v>343.02</v>
+      </c>
+      <c r="V32">
+        <v>9732</v>
+      </c>
+      <c r="W32">
+        <v>156</v>
+      </c>
+      <c r="X32">
+        <v>3744</v>
+      </c>
+      <c r="Y32">
+        <v>13632</v>
+      </c>
+      <c r="Z32" s="17">
+        <v>3540</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="2"/>
+      <c r="M33" s="15"/>
+    </row>
+    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L34" s="2"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L35" s="2"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L36" s="2"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
         <v>45</v>
       </c>
-      <c r="O37">
+      <c r="L38">
         <v>120000000</v>
       </c>
     </row>
-    <row r="38" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K38" t="s">
+    <row r="39" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
         <v>62</v>
       </c>
-      <c r="O38">
-        <f>O37/10^6</f>
+      <c r="L39">
+        <f>L38/10^6</f>
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="P41" s="1"/>
+    <row r="41" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M42" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="O4:Q4"/>
-  </mergeCells>
+  <autoFilter ref="A5:AA32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -8299,10 +8601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C44"/>
+  <dimension ref="B1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8312,7 +8614,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="18" t="s">
         <v>108</v>
       </c>
     </row>
@@ -8328,89 +8630,124 @@
       <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="26">
-        <f>'Switch test (2)'!S9</f>
-        <v>1.671422719069704E-2</v>
+      <c r="C4" s="15">
+        <f>'Switch test (2)'!O14</f>
+        <v>1.7000000000000015E-2</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="26">
-        <f>'Switch test (2)'!S17</f>
-        <v>0.24289637126776947</v>
+      <c r="C5" s="15">
+        <f>'Switch test (2)'!O22</f>
+        <v>0.20849999999999999</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="26">
-        <f>'Switch test (2)'!S29</f>
-        <v>2.7730597900987055</v>
+        <v>94</v>
+      </c>
+      <c r="C6" s="15">
+        <f>'Switch test (2)'!O28</f>
+        <v>2.5034999999999998</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="26">
-        <f>'Switch test (2)'!S26</f>
-        <v>2.8183070993637798</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="15">
+        <f>'Switch test (2)'!O32</f>
+        <v>2.8584999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>64</v>
       </c>
       <c r="C22">
-        <f>'Switch test (2)'!AA9</f>
+        <f>'Switch test (2)'!W14</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="O22" t="str">
+        <f>B4</f>
+        <v>Protothreads</v>
+      </c>
+      <c r="P22">
+        <f>C4</f>
+        <v>1.7000000000000015E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2">
-        <f>'Switch test (2)'!AA17</f>
+        <f>'Switch test (2)'!W22</f>
         <v>148</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="O23" t="str">
+        <f t="shared" ref="O23:P25" si="0">B5</f>
+        <v>Coroutines</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>0.20849999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="2">
+        <f>'Switch test (2)'!W28</f>
+        <v>144</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="0"/>
+        <v>FreeRTOS</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="0"/>
+        <v>2.5034999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="2">
-        <f>'Switch test (2)'!AA29</f>
+      <c r="C25" s="2">
+        <f>'Switch test (2)'!W32</f>
         <v>156</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="2">
-        <f>'Switch test (2)'!AA26</f>
-        <v>152</v>
+      <c r="O25" t="str">
+        <f t="shared" si="0"/>
+        <v>MQX Lite</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>2.8584999999999998</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="18" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8427,7 +8764,7 @@
         <v>64</v>
       </c>
       <c r="C41">
-        <f>'Switch test (2)'!Z9</f>
+        <f>'Switch test (2)'!V9</f>
         <v>4384</v>
       </c>
     </row>
@@ -8436,7 +8773,7 @@
         <v>65</v>
       </c>
       <c r="C42" s="2">
-        <f>'Switch test (2)'!Z17</f>
+        <f>'Switch test (2)'!V17</f>
         <v>6236</v>
       </c>
     </row>
@@ -8445,7 +8782,7 @@
         <v>95</v>
       </c>
       <c r="C43" s="2">
-        <f>'Switch test (2)'!Z29</f>
+        <f>'Switch test (2)'!V30</f>
         <v>8644</v>
       </c>
     </row>
@@ -8454,7 +8791,7 @@
         <v>94</v>
       </c>
       <c r="C44" s="2">
-        <f>'Switch test (2)'!Z26</f>
+        <f>'Switch test (2)'!V26</f>
         <v>6768</v>
       </c>
     </row>
@@ -8462,6 +8799,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" rightToLeft="1">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Charts (Switch test)'!P22:P22</xm:f>
+              <xm:sqref>Q22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Charts (Switch test)'!P23:P23</xm:f>
+              <xm:sqref>Q23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Charts (Switch test)'!P24:P24</xm:f>
+              <xm:sqref>Q24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Charts (Switch test)'!P25:P25</xm:f>
+              <xm:sqref>Q25</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Removed stqale code - tested <array> performance
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Switch test (1)" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Switch test (2)'!$A$5:$AA$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Switch test (2)'!$A$5:$AA$33</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -71,7 +71,7 @@
     <author>Bruce Belson</author>
   </authors>
   <commentList>
-    <comment ref="D24" authorId="0" shapeId="0">
+    <comment ref="D25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="126">
   <si>
     <t>Version</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>Time for context switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEDULER_USE_STL_ARRAY </t>
   </si>
 </sst>
 </file>
@@ -1124,11 +1127,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="491268744"/>
-        <c:axId val="491269136"/>
+        <c:axId val="246600976"/>
+        <c:axId val="246601360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="491268744"/>
+        <c:axId val="246600976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1174,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491269136"/>
+        <c:crossAx val="246601360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1179,7 +1182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="491269136"/>
+        <c:axId val="246601360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491268744"/>
+        <c:crossAx val="246600976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1492,11 +1495,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="491269920"/>
-        <c:axId val="491270312"/>
+        <c:axId val="210285872"/>
+        <c:axId val="210286264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="491269920"/>
+        <c:axId val="210285872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,7 +1542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491270312"/>
+        <c:crossAx val="210286264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1547,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="491270312"/>
+        <c:axId val="210286264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1654,7 +1657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491269920"/>
+        <c:crossAx val="210285872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1859,11 +1862,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="491271096"/>
-        <c:axId val="491271488"/>
+        <c:axId val="210287048"/>
+        <c:axId val="210287440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="491271096"/>
+        <c:axId val="210287048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1909,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491271488"/>
+        <c:crossAx val="210287440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1914,7 +1917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="491271488"/>
+        <c:axId val="210287440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,7 +2023,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491271096"/>
+        <c:crossAx val="210287048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2228,11 +2231,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="491272272"/>
-        <c:axId val="491272664"/>
+        <c:axId val="210289792"/>
+        <c:axId val="210290184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="491272272"/>
+        <c:axId val="210289792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2275,7 +2278,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491272664"/>
+        <c:crossAx val="210290184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2283,7 +2286,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="491272664"/>
+        <c:axId val="210290184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2390,7 +2393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491272272"/>
+        <c:crossAx val="210289792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2598,11 +2601,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="495296168"/>
-        <c:axId val="495296560"/>
+        <c:axId val="210291360"/>
+        <c:axId val="245847912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="495296168"/>
+        <c:axId val="210291360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2645,7 +2648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495296560"/>
+        <c:crossAx val="245847912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2653,7 +2656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="495296560"/>
+        <c:axId val="245847912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2760,7 +2763,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495296168"/>
+        <c:crossAx val="210291360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6900,13 +6903,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA42"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="W26" sqref="W26"/>
+      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7103,7 +7106,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N6" s="2" t="e">
-        <f t="shared" ref="N6:N20" si="0">M6*$L$39</f>
+        <f t="shared" ref="N6:N20" si="0">M6*$L$40</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7222,7 +7225,7 @@
         <v>1.671422719069704E-2</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" ref="P9" si="2">O9*$L$39</f>
+        <f t="shared" ref="P9" si="2">O9*$L$40</f>
         <v>2.0057072628836448</v>
       </c>
       <c r="V9">
@@ -7424,7 +7427,7 @@
         <v>0.14149999999999999</v>
       </c>
       <c r="S13" s="11">
-        <f>R13*$L$39</f>
+        <f>R13*$L$40</f>
         <v>16.979999999999997</v>
       </c>
       <c r="V13">
@@ -7488,7 +7491,7 @@
         <v>1.7000000000000015E-2</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" ref="P14" si="3">O14*$L$39</f>
+        <f t="shared" ref="P14" si="3">O14*$L$40</f>
         <v>2.0400000000000018</v>
       </c>
       <c r="R14" s="13">
@@ -7496,7 +7499,7 @@
         <v>0.1585</v>
       </c>
       <c r="S14" s="12">
-        <f>R14*$L$39</f>
+        <f>R14*$L$40</f>
         <v>19.02</v>
       </c>
       <c r="T14" s="15">
@@ -7504,7 +7507,7 @@
         <v>1.7000000000000015E-2</v>
       </c>
       <c r="U14">
-        <f>T14*$L$39</f>
+        <f>T14*$L$40</f>
         <v>2.0400000000000018</v>
       </c>
       <c r="V14">
@@ -7562,7 +7565,7 @@
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="10">
-        <f>R15*$L$39</f>
+        <f>R15*$L$40</f>
         <v>0</v>
       </c>
       <c r="V15">
@@ -7666,7 +7669,7 @@
         <v>0.24289637126776947</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" ref="P17:P18" si="5">O17*$L$39</f>
+        <f t="shared" ref="P17:P18" si="5">O17*$L$40</f>
         <v>29.147564552132337</v>
       </c>
       <c r="R17" s="1" t="e">
@@ -7674,7 +7677,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S17" s="12" t="e">
-        <f>R17*$L$39</f>
+        <f>R17*$L$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V17">
@@ -7858,7 +7861,7 @@
       <c r="M21" s="15"/>
       <c r="R21" s="1"/>
       <c r="S21" s="2">
-        <f>R21*$L$39</f>
+        <f>R21*$L$40</f>
         <v>0</v>
       </c>
     </row>
@@ -7899,7 +7902,7 @@
         <v>0.35</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" ref="N22" si="6">M22*$L$39</f>
+        <f t="shared" ref="N22:N24" si="6">M22*$L$40</f>
         <v>42</v>
       </c>
       <c r="O22" s="15">
@@ -7907,7 +7910,7 @@
         <v>0.20849999999999999</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" ref="P22" si="7">O22*$L$39</f>
+        <f t="shared" ref="P22" si="7">O22*$L$40</f>
         <v>25.02</v>
       </c>
       <c r="R22" s="13">
@@ -7915,7 +7918,7 @@
         <v>0.35</v>
       </c>
       <c r="S22" s="12">
-        <f>R22*$L$39</f>
+        <f>R22*$L$40</f>
         <v>42</v>
       </c>
       <c r="T22" s="15">
@@ -7923,7 +7926,7 @@
         <v>0.20849999999999999</v>
       </c>
       <c r="U22">
-        <f>T22*$L$39</f>
+        <f>T22*$L$40</f>
         <v>25.02</v>
       </c>
       <c r="V22">
@@ -7976,12 +7979,12 @@
       <c r="L23" s="2"/>
       <c r="M23" s="16"/>
       <c r="N23" s="10">
-        <f>M23*$L$39</f>
+        <f>M23*$L$40</f>
         <v>0</v>
       </c>
       <c r="R23" s="13"/>
       <c r="S23" s="10">
-        <f t="shared" ref="S23" si="8">R23*$L$39</f>
+        <f t="shared" ref="S23" si="8">R23*$L$40</f>
         <v>0</v>
       </c>
       <c r="V23">
@@ -8008,16 +8011,16 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -8035,25 +8038,32 @@
         <v>40</v>
       </c>
       <c r="L24" s="2"/>
-      <c r="M24" s="15"/>
+      <c r="M24" s="16">
+        <f>3.48/2</f>
+        <v>1.74</v>
+      </c>
+      <c r="N24" s="10">
+        <f>M24*$L$40</f>
+        <v>208.8</v>
+      </c>
       <c r="R24" s="13"/>
-      <c r="S24" s="12">
-        <f>R24*$L$39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
       </c>
       <c r="E25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -8065,24 +8075,20 @@
         <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L25" s="2">
-        <v>203100</v>
-      </c>
-      <c r="M25" s="15">
-        <f t="shared" ref="M25" si="9">10^6/L25</f>
-        <v>4.9236829148202856</v>
-      </c>
-      <c r="N25" s="2">
-        <f t="shared" ref="N25" si="10">M25*$L$39</f>
-        <v>590.84194977843424</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="15"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="12">
+        <f>R25*$L$40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>90</v>
       </c>
@@ -8108,52 +8114,26 @@
         <v>1</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L26" s="2">
-        <v>333998</v>
+        <v>203100</v>
       </c>
       <c r="M26" s="15">
-        <f t="shared" ref="M26:M29" si="11">10^6/L26</f>
-        <v>2.9940299043706848</v>
+        <f t="shared" ref="M26" si="9">10^6/L26</f>
+        <v>4.9236829148202856</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" ref="N26:N29" si="12">M26*$L$39</f>
-        <v>359.28358852448218</v>
-      </c>
-      <c r="O26" s="15">
-        <f>M26-M7</f>
-        <v>2.8183070993637798</v>
-      </c>
-      <c r="P26" s="2">
-        <f t="shared" ref="P26:P32" si="13">O26*$L$39</f>
-        <v>338.19685192365358</v>
-      </c>
-      <c r="V26">
-        <v>6768</v>
-      </c>
-      <c r="W26">
-        <v>152</v>
-      </c>
-      <c r="X26">
-        <v>4344</v>
-      </c>
-      <c r="Y26">
-        <v>11264</v>
-      </c>
-      <c r="Z26" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="N26" si="10">M26*$L$40</f>
+        <v>590.84194977843424</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -8177,49 +8157,46 @@
         <v>40</v>
       </c>
       <c r="L27" s="2">
-        <v>340668</v>
+        <v>333998</v>
       </c>
       <c r="M27" s="15">
-        <f t="shared" ref="M27" si="14">10^6/L27</f>
-        <v>2.9354092547582984</v>
+        <f t="shared" ref="M27:M30" si="11">10^6/L27</f>
+        <v>2.9940299043706848</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" ref="N27:N28" si="15">M27*$L$39</f>
-        <v>352.24911057099581</v>
+        <f t="shared" ref="N27:N30" si="12">M27*$L$40</f>
+        <v>359.28358852448218</v>
       </c>
       <c r="O27" s="15">
         <f>M27-M7</f>
-        <v>2.7596864497513933</v>
+        <v>2.8183070993637798</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" ref="P27:P28" si="16">O27*$L$39</f>
-        <v>331.16237397016721</v>
+        <f t="shared" ref="P27:P33" si="13">O27*$L$40</f>
+        <v>338.19685192365358</v>
       </c>
       <c r="V27">
-        <v>7856</v>
+        <v>6768</v>
       </c>
       <c r="W27">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="X27">
         <v>4344</v>
       </c>
       <c r="Y27">
-        <v>12344</v>
-      </c>
-      <c r="Z27" s="17">
-        <v>3038</v>
+        <v>11264</v>
+      </c>
+      <c r="Z27" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="AA27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="b">
-        <v>1</v>
-      </c>
+    <row r="28" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
         <v>52</v>
@@ -8245,354 +8222,423 @@
       <c r="K28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="16">
+      <c r="L28" s="2">
+        <v>340668</v>
+      </c>
+      <c r="M28" s="15">
+        <f t="shared" ref="M28" si="14">10^6/L28</f>
+        <v>2.9354092547582984</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" ref="N28:N29" si="15">M28*$L$40</f>
+        <v>352.24911057099581</v>
+      </c>
+      <c r="O28" s="15">
+        <f>M28-M7</f>
+        <v>2.7596864497513933</v>
+      </c>
+      <c r="P28" s="2">
+        <f t="shared" ref="P28:P29" si="16">O28*$L$40</f>
+        <v>331.16237397016721</v>
+      </c>
+      <c r="V28">
+        <v>7856</v>
+      </c>
+      <c r="W28">
+        <v>144</v>
+      </c>
+      <c r="X28">
+        <v>4344</v>
+      </c>
+      <c r="Y28">
+        <v>12344</v>
+      </c>
+      <c r="Z28" s="17">
+        <v>3038</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="16">
         <f>5.29/2</f>
         <v>2.645</v>
       </c>
-      <c r="N28" s="12">
+      <c r="N29" s="12">
         <f t="shared" si="15"/>
         <v>317.39999999999998</v>
       </c>
-      <c r="O28" s="15">
-        <f>M28-M$13</f>
+      <c r="O29" s="15">
+        <f>M29-M$13</f>
         <v>2.5034999999999998</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P29" s="1">
         <f t="shared" si="16"/>
         <v>300.41999999999996</v>
       </c>
-      <c r="R28" s="13">
+      <c r="R29" s="13">
         <f>5.29/2</f>
         <v>2.645</v>
       </c>
-      <c r="S28" s="12">
-        <f>R28*$L$39</f>
+      <c r="S29" s="12">
+        <f>R29*$L$40</f>
         <v>317.39999999999998</v>
       </c>
-      <c r="T28" s="15">
-        <f>R28-R$13</f>
+      <c r="T29" s="15">
+        <f>R29-R$13</f>
         <v>2.5034999999999998</v>
       </c>
-      <c r="U28">
-        <f>T28*$L$39</f>
+      <c r="U29">
+        <f>T29*$L$40</f>
         <v>300.41999999999996</v>
       </c>
-      <c r="V28">
+      <c r="V29">
         <v>6676</v>
       </c>
-      <c r="W28">
+      <c r="W29">
         <v>144</v>
       </c>
-      <c r="X28">
+      <c r="X29">
         <v>4284</v>
       </c>
-      <c r="Y28">
+      <c r="Y29">
         <v>11104</v>
       </c>
-      <c r="Z28" s="17" t="s">
+      <c r="Z29" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AA29" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="30" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>92</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>91</v>
       </c>
-      <c r="E29" t="b">
-        <v>0</v>
-      </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29">
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30">
         <v>2</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29" s="6" t="s">
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L30" s="2">
         <v>242656</v>
       </c>
-      <c r="M29" s="15">
+      <c r="M30" s="15">
         <f t="shared" si="11"/>
         <v>4.121060266385336</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N30" s="2">
         <f t="shared" si="12"/>
         <v>494.52723196624032</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>92</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>91</v>
       </c>
-      <c r="E30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30">
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31">
         <v>2</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" s="6" t="s">
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L31" s="2">
         <v>339123</v>
       </c>
-      <c r="M30" s="15">
-        <f t="shared" ref="M30" si="17">10^6/L30</f>
+      <c r="M31" s="15">
+        <f t="shared" ref="M31" si="17">10^6/L31</f>
         <v>2.9487825951056106</v>
       </c>
-      <c r="N30" s="2">
-        <f t="shared" ref="N30" si="18">M30*$L$39</f>
+      <c r="N31" s="2">
+        <f t="shared" ref="N31" si="18">M31*$L$40</f>
         <v>353.85391141267326</v>
       </c>
-      <c r="O30" s="15">
-        <f>M30-M7</f>
+      <c r="O31" s="15">
+        <f>M31-M7</f>
         <v>2.7730597900987055</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P31" s="2">
         <f t="shared" si="13"/>
         <v>332.76717481184465</v>
       </c>
-      <c r="V30">
+      <c r="V31">
         <v>8644</v>
       </c>
-      <c r="W30">
+      <c r="W31">
         <v>156</v>
       </c>
-      <c r="X30">
+      <c r="X31">
         <v>4328</v>
       </c>
-      <c r="Y30">
+      <c r="Y31">
         <v>13128</v>
       </c>
-      <c r="Z30" s="17">
+      <c r="Z31" s="17">
         <v>3348</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AA31" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+    <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>92</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>52</v>
       </c>
-      <c r="E31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31">
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32">
         <v>2</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" s="6" t="s">
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L32" s="2">
         <v>324856</v>
       </c>
-      <c r="M31" s="15">
-        <f t="shared" ref="M31" si="19">10^6/L31</f>
+      <c r="M32" s="15">
+        <f t="shared" ref="M32" si="19">10^6/L32</f>
         <v>3.0782869948531042</v>
       </c>
-      <c r="N31" s="2">
-        <f t="shared" ref="N31" si="20">M31*$L$39</f>
+      <c r="N32" s="2">
+        <f t="shared" ref="N32" si="20">M32*$L$40</f>
         <v>369.39443938237252</v>
       </c>
-      <c r="O31" s="15">
-        <f>M31-M7</f>
+      <c r="O32" s="15">
+        <f>M32-M7</f>
         <v>2.9025641898461991</v>
       </c>
-      <c r="P31" s="2">
+      <c r="P32" s="2">
         <f t="shared" si="13"/>
         <v>348.30770278154387</v>
       </c>
-      <c r="V31">
+      <c r="V32">
         <v>11040</v>
       </c>
-      <c r="W31">
+      <c r="W32">
         <v>156</v>
       </c>
-      <c r="X31">
+      <c r="X32">
         <v>4332</v>
       </c>
-      <c r="Y31">
+      <c r="Y32">
         <v>15528</v>
       </c>
-      <c r="Z31" s="17" t="s">
+      <c r="Z32" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AA32" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="b">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="33" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
         <v>112</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>52</v>
       </c>
-      <c r="E32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32">
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <v>2</v>
       </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" s="6" t="s">
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L32" s="2"/>
-      <c r="M32" s="16">
+      <c r="L33" s="2"/>
+      <c r="M33" s="16">
         <f>6/2</f>
         <v>3</v>
       </c>
-      <c r="N32" s="10">
-        <f>M32*$L$39</f>
+      <c r="N33" s="10">
+        <f>M33*$L$40</f>
         <v>360</v>
       </c>
-      <c r="O32" s="15">
-        <f>M32-M$13</f>
+      <c r="O33" s="15">
+        <f>M33-M$13</f>
         <v>2.8584999999999998</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P33" s="1">
         <f t="shared" si="13"/>
         <v>343.02</v>
       </c>
-      <c r="R32" s="16">
+      <c r="R33" s="16">
         <f>6/2</f>
         <v>3</v>
       </c>
-      <c r="S32" s="12">
-        <f>R32*$L$39</f>
+      <c r="S33" s="12">
+        <f>R33*$L$40</f>
         <v>360</v>
       </c>
-      <c r="T32" s="15">
-        <f>R32-R$13</f>
+      <c r="T33" s="15">
+        <f>R33-R$13</f>
         <v>2.8584999999999998</v>
       </c>
-      <c r="U32">
-        <f>T32*$L$39</f>
+      <c r="U33">
+        <f>T33*$L$40</f>
         <v>343.02</v>
       </c>
-      <c r="V32">
+      <c r="V33">
         <v>9732</v>
       </c>
-      <c r="W32">
+      <c r="W33">
         <v>156</v>
       </c>
-      <c r="X32">
+      <c r="X33">
         <v>3744</v>
       </c>
-      <c r="Y32">
+      <c r="Y33">
         <v>13632</v>
       </c>
-      <c r="Z32" s="17">
+      <c r="Z33" s="17">
         <v>3540</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AA33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="11:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L33" s="2"/>
-      <c r="M33" s="15"/>
-    </row>
-    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L34" s="2"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="15"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="L36" s="2"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K38" t="s">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L37" s="2"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
         <v>45</v>
       </c>
-      <c r="L38">
+      <c r="L39">
         <v>120000000</v>
       </c>
     </row>
-    <row r="39" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K39" t="s">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
         <v>62</v>
       </c>
-      <c r="L39">
-        <f>L38/10^6</f>
+      <c r="L40">
+        <f>L39/10^6</f>
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="M42" s="1"/>
     </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M43" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A5:AA32"/>
+  <autoFilter ref="A5:AA33"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -8603,7 +8649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -8649,7 +8695,7 @@
         <v>94</v>
       </c>
       <c r="C6" s="15">
-        <f>'Switch test (2)'!O28</f>
+        <f>'Switch test (2)'!O29</f>
         <v>2.5034999999999998</v>
       </c>
     </row>
@@ -8658,7 +8704,7 @@
         <v>95</v>
       </c>
       <c r="C7" s="15">
-        <f>'Switch test (2)'!O32</f>
+        <f>'Switch test (2)'!O33</f>
         <v>2.8584999999999998</v>
       </c>
     </row>
@@ -8717,7 +8763,7 @@
         <v>94</v>
       </c>
       <c r="C24" s="2">
-        <f>'Switch test (2)'!W28</f>
+        <f>'Switch test (2)'!W29</f>
         <v>144</v>
       </c>
       <c r="O24" t="str">
@@ -8734,7 +8780,7 @@
         <v>95</v>
       </c>
       <c r="C25" s="2">
-        <f>'Switch test (2)'!W32</f>
+        <f>'Switch test (2)'!W33</f>
         <v>156</v>
       </c>
       <c r="O25" t="str">
@@ -8782,7 +8828,7 @@
         <v>95</v>
       </c>
       <c r="C43" s="2">
-        <f>'Switch test (2)'!V30</f>
+        <f>'Switch test (2)'!V31</f>
         <v>8644</v>
       </c>
     </row>
@@ -8791,7 +8837,7 @@
         <v>94</v>
       </c>
       <c r="C44" s="2">
-        <f>'Switch test (2)'!V26</f>
+        <f>'Switch test (2)'!V27</f>
         <v>6768</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Built with preallocated per-task frames
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="127">
   <si>
     <t>Version</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t xml:space="preserve">SCHEDULER_USE_STL_ARRAY </t>
+  </si>
+  <si>
+    <t>coroinc_xt</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1058,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1127,11 +1129,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="246600976"/>
-        <c:axId val="246601360"/>
+        <c:axId val="234634536"/>
+        <c:axId val="234634928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246600976"/>
+        <c:axId val="234634536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246601360"/>
+        <c:crossAx val="234634928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1182,7 +1184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246601360"/>
+        <c:axId val="234634928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1230,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1289,7 +1290,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246600976"/>
+        <c:crossAx val="234634536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1423,7 +1424,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1495,11 +1495,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="210285872"/>
-        <c:axId val="210286264"/>
+        <c:axId val="234635712"/>
+        <c:axId val="234636104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210285872"/>
+        <c:axId val="234635712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1542,7 +1542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210286264"/>
+        <c:crossAx val="234636104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1550,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210286264"/>
+        <c:axId val="234636104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1596,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1657,7 +1656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210285872"/>
+        <c:crossAx val="234635712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1862,11 +1861,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="210287048"/>
-        <c:axId val="210287440"/>
+        <c:axId val="339435056"/>
+        <c:axId val="339435448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210287048"/>
+        <c:axId val="339435056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210287440"/>
+        <c:crossAx val="339435448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1917,7 +1916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210287440"/>
+        <c:axId val="339435448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2023,7 +2022,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210287048"/>
+        <c:crossAx val="339435056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2159,7 +2158,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2231,11 +2229,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="210289792"/>
-        <c:axId val="210290184"/>
+        <c:axId val="339436232"/>
+        <c:axId val="339436624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210289792"/>
+        <c:axId val="339436232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210290184"/>
+        <c:crossAx val="339436624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2286,7 +2284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210290184"/>
+        <c:axId val="339436624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2330,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2393,7 +2390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210289792"/>
+        <c:crossAx val="339436232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2529,7 +2526,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2601,11 +2597,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="210291360"/>
-        <c:axId val="245847912"/>
+        <c:axId val="339437800"/>
+        <c:axId val="339438192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210291360"/>
+        <c:axId val="339437800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2648,7 +2644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245847912"/>
+        <c:crossAx val="339438192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2656,7 +2652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245847912"/>
+        <c:axId val="339438192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2702,7 +2698,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2763,7 +2758,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210291360"/>
+        <c:crossAx val="339437800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5823,8 +5818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6906,10 +6901,10 @@
   <dimension ref="A1:AA43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomRight" activeCell="R34" sqref="R34:S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7902,7 +7897,7 @@
         <v>0.35</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" ref="N22:N24" si="6">M22*$L$40</f>
+        <f t="shared" ref="N22" si="6">M22*$L$40</f>
         <v>42</v>
       </c>
       <c r="O22" s="15">
@@ -8598,11 +8593,48 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="L34" s="2"/>
-      <c r="M34" s="15"/>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M34" s="16"/>
+      <c r="N34" s="10"/>
+      <c r="R34" s="16">
+        <f>3.48/2</f>
+        <v>1.74</v>
+      </c>
+      <c r="S34" s="10">
+        <f>R34*21</f>
+        <v>36.54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
     </row>

</xml_diff>

<commit_message>
O1 tests to comapre with CoroInC
</commit_message>
<xml_diff>
--- a/Comparisons.xlsx
+++ b/Comparisons.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="133">
   <si>
     <t>Version</t>
   </si>
@@ -545,15 +545,34 @@
   <si>
     <t>coroinc_xt</t>
   </si>
+  <si>
+    <t>Slow clock 21 MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   267c</t>
+  </si>
+  <si>
+    <t>coroinc_xt.elf</t>
+  </si>
+  <si>
+    <t>DebugLLVM_NSO1</t>
+  </si>
+  <si>
+    <t>Does not build</t>
+  </si>
+  <si>
+    <t>DebugLLVMO1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,8 +653,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,6 +711,16 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -859,7 +902,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -871,8 +914,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -946,13 +991,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="11" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="12" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="8" builtinId="34"/>
     <cellStyle name="20% - Accent4" xfId="9" builtinId="42"/>
+    <cellStyle name="Bad" xfId="12" builtinId="27"/>
     <cellStyle name="Calculation" xfId="10" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
+    <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="5" builtinId="10"/>
@@ -6898,13 +6952,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA43"/>
+  <dimension ref="A1:AA45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="I18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R34" sqref="R34:S34"/>
+      <selection pane="bottomRight" activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7101,7 +7155,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N6" s="2" t="e">
-        <f t="shared" ref="N6:N20" si="0">M6*$L$40</f>
+        <f>M6*$L$42</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7141,7 +7195,7 @@
         <v>0.17572280500690501</v>
       </c>
       <c r="N7" s="11">
-        <f t="shared" si="0"/>
+        <f>M7*$L$42</f>
         <v>21.086736600828601</v>
       </c>
     </row>
@@ -7171,11 +7225,11 @@
         <v>44</v>
       </c>
       <c r="M8" s="15" t="e">
-        <f t="shared" ref="M8:M12" si="1">10^6/L8</f>
+        <f t="shared" ref="M8:M12" si="0">10^6/L8</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N8" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f>M8*$L$42</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7208,11 +7262,11 @@
         <v>5196505</v>
       </c>
       <c r="M9" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.19243703219760205</v>
       </c>
       <c r="N9" s="12">
-        <f t="shared" si="0"/>
+        <f>M9*$L$42</f>
         <v>23.092443863712248</v>
       </c>
       <c r="O9" s="15">
@@ -7220,7 +7274,7 @@
         <v>1.671422719069704E-2</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" ref="P9" si="2">O9*$L$40</f>
+        <f>O9*$L$42</f>
         <v>2.0057072628836448</v>
       </c>
       <c r="V9">
@@ -7274,11 +7328,11 @@
         <v>609794</v>
       </c>
       <c r="M10" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6398980639363456</v>
       </c>
       <c r="N10" s="10">
-        <f t="shared" si="0"/>
+        <f>M10*$L$42</f>
         <v>196.78776767236147</v>
       </c>
       <c r="V10">
@@ -7332,13 +7386,13 @@
         <v>40</v>
       </c>
       <c r="M11" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="N11" s="2" t="e">
+        <f>M11*$L$42</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -7372,11 +7426,11 @@
         <v>40</v>
       </c>
       <c r="M12" s="15" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f>M12*$L$42</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7414,7 +7468,7 @@
         <v>0.14149999999999999</v>
       </c>
       <c r="N13" s="11">
-        <f t="shared" si="0"/>
+        <f>M13*$L$42</f>
         <v>16.979999999999997</v>
       </c>
       <c r="R13" s="16">
@@ -7422,7 +7476,7 @@
         <v>0.14149999999999999</v>
       </c>
       <c r="S13" s="11">
-        <f>R13*$L$40</f>
+        <f>R13*$L$42</f>
         <v>16.979999999999997</v>
       </c>
       <c r="V13">
@@ -7478,7 +7532,7 @@
         <v>0.1585</v>
       </c>
       <c r="N14" s="12">
-        <f t="shared" si="0"/>
+        <f>M14*$L$42</f>
         <v>19.02</v>
       </c>
       <c r="O14" s="15">
@@ -7486,7 +7540,7 @@
         <v>1.7000000000000015E-2</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" ref="P14" si="3">O14*$L$40</f>
+        <f>O14*$L$42</f>
         <v>2.0400000000000018</v>
       </c>
       <c r="R14" s="13">
@@ -7494,7 +7548,7 @@
         <v>0.1585</v>
       </c>
       <c r="S14" s="12">
-        <f>R14*$L$40</f>
+        <f>R14*$L$42</f>
         <v>19.02</v>
       </c>
       <c r="T14" s="15">
@@ -7502,7 +7556,7 @@
         <v>1.7000000000000015E-2</v>
       </c>
       <c r="U14">
-        <f>T14*$L$40</f>
+        <f>T14*$L$42</f>
         <v>2.0400000000000018</v>
       </c>
       <c r="V14">
@@ -7555,12 +7609,12 @@
       <c r="L15" s="2"/>
       <c r="M15" s="16"/>
       <c r="N15" s="10">
-        <f t="shared" si="0"/>
+        <f>M15*$L$42</f>
         <v>0</v>
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="10">
-        <f>R15*$L$40</f>
+        <f>R15*$L$42</f>
         <v>0</v>
       </c>
       <c r="V15">
@@ -7612,11 +7666,11 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="15" t="e">
-        <f t="shared" ref="M16:M20" si="4">10^6/L16</f>
+        <f t="shared" ref="M16:M20" si="1">10^6/L16</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N16" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f>M16*$L$42</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7652,11 +7706,11 @@
         <v>2388806</v>
       </c>
       <c r="M17" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0.41861917627467449</v>
       </c>
       <c r="N17" s="12">
-        <f t="shared" si="0"/>
+        <f>M17*$L$42</f>
         <v>50.234301152960938</v>
       </c>
       <c r="O17" s="15">
@@ -7664,7 +7718,7 @@
         <v>0.24289637126776947</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" ref="P17:P18" si="5">O17*$L$40</f>
+        <f t="shared" ref="P17:P18" si="2">O17*$L$42</f>
         <v>29.147564552132337</v>
       </c>
       <c r="R17" s="1" t="e">
@@ -7672,7 +7726,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S17" s="12" t="e">
-        <f>R17*$L$40</f>
+        <f>R17*$L$42</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V17">
@@ -7726,11 +7780,11 @@
         <v>538043</v>
       </c>
       <c r="M18" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1.8585875106636458</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="0"/>
+        <f>M18*$L$42</f>
         <v>223.03050127963749</v>
       </c>
       <c r="O18" s="15">
@@ -7738,7 +7792,7 @@
         <v>0.21868944672730017</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>26.242733607276023</v>
       </c>
     </row>
@@ -7775,11 +7829,11 @@
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="15" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N19" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f>M19*$L$42</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7816,11 +7870,11 @@
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="15" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N20" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f>M20*$L$42</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7856,7 +7910,7 @@
       <c r="M21" s="15"/>
       <c r="R21" s="1"/>
       <c r="S21" s="2">
-        <f>R21*$L$40</f>
+        <f>R21*$L$42</f>
         <v>0</v>
       </c>
     </row>
@@ -7897,7 +7951,7 @@
         <v>0.35</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" ref="N22" si="6">M22*$L$40</f>
+        <f t="shared" ref="N22" si="3">M22*$L$42</f>
         <v>42</v>
       </c>
       <c r="O22" s="15">
@@ -7905,7 +7959,7 @@
         <v>0.20849999999999999</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" ref="P22" si="7">O22*$L$40</f>
+        <f t="shared" ref="P22" si="4">O22*$L$42</f>
         <v>25.02</v>
       </c>
       <c r="R22" s="13">
@@ -7913,7 +7967,7 @@
         <v>0.35</v>
       </c>
       <c r="S22" s="12">
-        <f>R22*$L$40</f>
+        <f>R22*$L$42</f>
         <v>42</v>
       </c>
       <c r="T22" s="15">
@@ -7921,7 +7975,7 @@
         <v>0.20849999999999999</v>
       </c>
       <c r="U22">
-        <f>T22*$L$40</f>
+        <f>T22*$L$42</f>
         <v>25.02</v>
       </c>
       <c r="V22">
@@ -7974,12 +8028,12 @@
       <c r="L23" s="2"/>
       <c r="M23" s="16"/>
       <c r="N23" s="10">
-        <f>M23*$L$40</f>
+        <f>M23*$L$42</f>
         <v>0</v>
       </c>
       <c r="R23" s="13"/>
       <c r="S23" s="10">
-        <f t="shared" ref="S23" si="8">R23*$L$40</f>
+        <f t="shared" ref="S23" si="5">R23*$L$42</f>
         <v>0</v>
       </c>
       <c r="V23">
@@ -8038,7 +8092,7 @@
         <v>1.74</v>
       </c>
       <c r="N24" s="10">
-        <f>M24*$L$40</f>
+        <f>M24*$L$42</f>
         <v>208.8</v>
       </c>
       <c r="R24" s="13"/>
@@ -8079,7 +8133,7 @@
       <c r="M25" s="15"/>
       <c r="R25" s="13"/>
       <c r="S25" s="12">
-        <f>R25*$L$40</f>
+        <f>R25*$L$42</f>
         <v>0</v>
       </c>
     </row>
@@ -8115,11 +8169,11 @@
         <v>203100</v>
       </c>
       <c r="M26" s="15">
-        <f t="shared" ref="M26" si="9">10^6/L26</f>
+        <f t="shared" ref="M26" si="6">10^6/L26</f>
         <v>4.9236829148202856</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" ref="N26" si="10">M26*$L$40</f>
+        <f t="shared" ref="N26" si="7">M26*$L$42</f>
         <v>590.84194977843424</v>
       </c>
     </row>
@@ -8155,11 +8209,11 @@
         <v>333998</v>
       </c>
       <c r="M27" s="15">
-        <f t="shared" ref="M27:M30" si="11">10^6/L27</f>
+        <f t="shared" ref="M27:M30" si="8">10^6/L27</f>
         <v>2.9940299043706848</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" ref="N27:N30" si="12">M27*$L$40</f>
+        <f t="shared" ref="N27:N30" si="9">M27*$L$42</f>
         <v>359.28358852448218</v>
       </c>
       <c r="O27" s="15">
@@ -8167,7 +8221,7 @@
         <v>2.8183070993637798</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" ref="P27:P33" si="13">O27*$L$40</f>
+        <f t="shared" ref="P27:P33" si="10">O27*$L$42</f>
         <v>338.19685192365358</v>
       </c>
       <c r="V27">
@@ -8221,11 +8275,11 @@
         <v>340668</v>
       </c>
       <c r="M28" s="15">
-        <f t="shared" ref="M28" si="14">10^6/L28</f>
+        <f t="shared" ref="M28" si="11">10^6/L28</f>
         <v>2.9354092547582984</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" ref="N28:N29" si="15">M28*$L$40</f>
+        <f t="shared" ref="N28:N29" si="12">M28*$L$42</f>
         <v>352.24911057099581</v>
       </c>
       <c r="O28" s="15">
@@ -8233,7 +8287,7 @@
         <v>2.7596864497513933</v>
       </c>
       <c r="P28" s="2">
-        <f t="shared" ref="P28:P29" si="16">O28*$L$40</f>
+        <f t="shared" ref="P28:P29" si="13">O28*$L$42</f>
         <v>331.16237397016721</v>
       </c>
       <c r="V28">
@@ -8292,7 +8346,7 @@
         <v>2.645</v>
       </c>
       <c r="N29" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>317.39999999999998</v>
       </c>
       <c r="O29" s="15">
@@ -8300,7 +8354,7 @@
         <v>2.5034999999999998</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>300.41999999999996</v>
       </c>
       <c r="R29" s="13">
@@ -8308,7 +8362,7 @@
         <v>2.645</v>
       </c>
       <c r="S29" s="12">
-        <f>R29*$L$40</f>
+        <f>R29*$L$42</f>
         <v>317.39999999999998</v>
       </c>
       <c r="T29" s="15">
@@ -8316,7 +8370,7 @@
         <v>2.5034999999999998</v>
       </c>
       <c r="U29">
-        <f>T29*$L$40</f>
+        <f>T29*$L$42</f>
         <v>300.41999999999996</v>
       </c>
       <c r="V29">
@@ -8370,11 +8424,11 @@
         <v>242656</v>
       </c>
       <c r="M30" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>4.121060266385336</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>494.52723196624032</v>
       </c>
     </row>
@@ -8410,11 +8464,11 @@
         <v>339123</v>
       </c>
       <c r="M31" s="15">
-        <f t="shared" ref="M31" si="17">10^6/L31</f>
+        <f t="shared" ref="M31" si="14">10^6/L31</f>
         <v>2.9487825951056106</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" ref="N31" si="18">M31*$L$40</f>
+        <f t="shared" ref="N31" si="15">M31*$L$42</f>
         <v>353.85391141267326</v>
       </c>
       <c r="O31" s="15">
@@ -8422,7 +8476,7 @@
         <v>2.7730597900987055</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>332.76717481184465</v>
       </c>
       <c r="V31">
@@ -8476,11 +8530,11 @@
         <v>324856</v>
       </c>
       <c r="M32" s="15">
-        <f t="shared" ref="M32" si="19">10^6/L32</f>
+        <f t="shared" ref="M32" si="16">10^6/L32</f>
         <v>3.0782869948531042</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" ref="N32" si="20">M32*$L$40</f>
+        <f t="shared" ref="N32" si="17">M32*$L$42</f>
         <v>369.39443938237252</v>
       </c>
       <c r="O32" s="15">
@@ -8488,7 +8542,7 @@
         <v>2.9025641898461991</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>348.30770278154387</v>
       </c>
       <c r="V32">
@@ -8547,7 +8601,7 @@
         <v>3</v>
       </c>
       <c r="N33" s="10">
-        <f>M33*$L$40</f>
+        <f>M33*$L$42</f>
         <v>360</v>
       </c>
       <c r="O33" s="15">
@@ -8555,7 +8609,7 @@
         <v>2.8584999999999998</v>
       </c>
       <c r="P33" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>343.02</v>
       </c>
       <c r="R33" s="16">
@@ -8563,7 +8617,7 @@
         <v>3</v>
       </c>
       <c r="S33" s="12">
-        <f>R33*$L$40</f>
+        <f>R33*$L$42</f>
         <v>360</v>
       </c>
       <c r="T33" s="15">
@@ -8571,7 +8625,7 @@
         <v>2.8584999999999998</v>
       </c>
       <c r="U33">
-        <f>T33*$L$40</f>
+        <f>T33*$L$42</f>
         <v>343.02</v>
       </c>
       <c r="V33">
@@ -8600,7 +8654,9 @@
       <c r="C34" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E34" t="b">
         <v>1</v>
       </c>
@@ -8625,49 +8681,277 @@
       <c r="L34" s="2"/>
       <c r="M34" s="16"/>
       <c r="N34" s="10"/>
-      <c r="R34" s="16">
+      <c r="R34">
         <f>3.48/2</f>
         <v>1.74</v>
       </c>
-      <c r="S34" s="10">
+      <c r="S34">
         <f>R34*21</f>
         <v>36.54</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R35" s="16">
+        <f>0.9835/2</f>
+        <v>0.49175000000000002</v>
+      </c>
+      <c r="S35" s="10">
+        <f>R35*$L$42</f>
+        <v>59.010000000000005</v>
+      </c>
+      <c r="T35" s="15">
+        <f>R35-R13</f>
+        <v>0.35025000000000006</v>
+      </c>
+      <c r="U35">
+        <f>T35*$L$42</f>
+        <v>42.030000000000008</v>
+      </c>
+      <c r="V35">
+        <v>8272</v>
+      </c>
+      <c r="W35">
+        <v>144</v>
+      </c>
+      <c r="X35">
+        <v>1436</v>
+      </c>
+      <c r="Y35">
+        <v>9852</v>
+      </c>
+      <c r="Z35" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" s="43" t="s">
+        <v>40</v>
+      </c>
       <c r="L36" s="2"/>
       <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R36" s="16"/>
+      <c r="S36" s="10"/>
+      <c r="V36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="L37" s="2"/>
       <c r="M37" s="1"/>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K39" t="s">
+      <c r="R37" s="13">
+        <f>0.75/2</f>
+        <v>0.375</v>
+      </c>
+      <c r="S37" s="12">
+        <f>R37*$L$42</f>
         <v>45</v>
       </c>
-      <c r="L39">
+      <c r="T37" s="42">
+        <f>R37-R13</f>
+        <v>0.23350000000000001</v>
+      </c>
+      <c r="U37">
+        <f>T37*$L$42</f>
+        <v>28.020000000000003</v>
+      </c>
+      <c r="V37">
+        <v>3004</v>
+      </c>
+      <c r="W37">
+        <v>148</v>
+      </c>
+      <c r="X37">
+        <v>1064</v>
+      </c>
+      <c r="Y37">
+        <v>4216</v>
+      </c>
+      <c r="Z37" s="17">
+        <v>1078</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="M38" s="1"/>
+      <c r="R38" s="13">
+        <f>6.15/2</f>
+        <v>3.0750000000000002</v>
+      </c>
+      <c r="S38" s="12">
+        <f>R38*$L$42</f>
+        <v>369</v>
+      </c>
+      <c r="T38" s="42">
+        <f>R38-R13</f>
+        <v>2.9335</v>
+      </c>
+      <c r="U38">
+        <f>T38*$L$42</f>
+        <v>352.02</v>
+      </c>
+      <c r="V38">
+        <v>6088</v>
+      </c>
+      <c r="W38">
+        <v>148</v>
+      </c>
+      <c r="X38">
+        <v>4284</v>
+      </c>
+      <c r="Y38">
+        <v>10520</v>
+      </c>
+      <c r="Z38" s="17">
+        <v>2918</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>45</v>
+      </c>
+      <c r="L41">
         <v>120000000</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K40" t="s">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
         <v>62</v>
       </c>
-      <c r="L40">
-        <f>L39/10^6</f>
+      <c r="L42">
+        <f>L41/10^6</f>
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M42" s="1"/>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M43" s="1"/>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M45" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:AA33"/>

</xml_diff>